<commit_message>
Added my review comments please do not remove them untill the code is reviewed successfully
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-AddCategory.xlsx
+++ b/tests/artifact/script/UI-AddCategory.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="906">
   <si>
     <t>target</t>
   </si>
@@ -2345,6 +2345,9 @@
     <t>3000</t>
   </si>
   <si>
+    <t>How it will verify the user has landed on the Category page&gt;</t>
+  </si>
+  <si>
     <t>click on Categories in Inventroy</t>
   </si>
   <si>
@@ -2621,6 +2624,9 @@
     <t>Search the created Category</t>
   </si>
   <si>
+    <t>Rework on the edit functionality and ask aditi how to verify edit functionality</t>
+  </si>
+  <si>
     <t>click on Edit button</t>
   </si>
   <si>
@@ -2736,6 +2742,9 @@
   </si>
   <si>
     <t>${ec.delete.tax.row.xpath}[${edittaxrowcount}]${ec.delete.spec.tax.button}</t>
+  </si>
+  <si>
+    <t>I see only element is being verified. Where is the message verification? The data is successfully deleted? Use expected and actual here</t>
   </si>
   <si>
     <t>Checking with Same Category name is creating or not</t>
@@ -2842,6 +2851,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Tahoma"/>
       <charset val="134"/>
@@ -2849,13 +2865,6 @@
     <font>
       <sz val="11"/>
       <name val="Consolas"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3639,15 +3648,19 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3665,10 +3678,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3700,7 +3709,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3792,7 +3801,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6978,13 +6987,13 @@
       <c r="B5" s="30" t="s">
         <v>748</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>447</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>749</v>
       </c>
       <c r="F5" s="63" t="s">
@@ -10169,8 +10178,8 @@
   <sheetPr/>
   <dimension ref="A1:O200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -10386,9 +10395,11 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A8" s="19"/>
+      <c r="A8" s="31" t="s">
+        <v>760</v>
+      </c>
       <c r="B8" s="30" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>30</v>
@@ -10397,7 +10408,7 @@
         <v>363</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
@@ -10412,22 +10423,22 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A9" s="19" t="s">
-        <v>762</v>
-      </c>
-      <c r="B9" s="31" t="s">
         <v>763</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="B9" s="32" t="s">
+        <v>764</v>
+      </c>
+      <c r="C9" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
@@ -10442,7 +10453,7 @@
     <row r="10" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A10" s="19"/>
       <c r="B10" s="30" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>30</v>
@@ -10451,10 +10462,10 @@
         <v>483</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
@@ -10469,19 +10480,19 @@
     <row r="11" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A11" s="19"/>
       <c r="B11" s="30" t="s">
-        <v>769</v>
-      </c>
-      <c r="C11" s="34" t="s">
+        <v>770</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="36" t="s">
         <v>471</v>
       </c>
-      <c r="E11" s="35" t="s">
-        <v>770</v>
-      </c>
-      <c r="F11" s="36" t="s">
+      <c r="E11" s="36" t="s">
         <v>771</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>772</v>
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
@@ -10496,17 +10507,17 @@
     <row r="12" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A12" s="19"/>
       <c r="B12" s="30"/>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="36" t="s">
         <v>465</v>
       </c>
-      <c r="E12" s="35" t="s">
-        <v>772</v>
-      </c>
-      <c r="F12" s="36" t="s">
+      <c r="E12" s="36" t="s">
         <v>773</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>774</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
@@ -10521,17 +10532,17 @@
     <row r="13" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A13" s="19"/>
       <c r="B13" s="30"/>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="35" t="s">
-        <v>774</v>
+      <c r="E13" s="36" t="s">
+        <v>775</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -10546,19 +10557,19 @@
     <row r="14" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="19"/>
       <c r="B14" s="30" t="s">
-        <v>776</v>
-      </c>
-      <c r="C14" s="34" t="s">
+        <v>777</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>770</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>777</v>
+      <c r="E14" s="36" t="s">
+        <v>771</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>778</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -10573,7 +10584,7 @@
     <row r="15" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A15" s="19"/>
       <c r="B15" s="30" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>30</v>
@@ -10582,10 +10593,10 @@
         <v>493</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -10600,19 +10611,19 @@
     <row r="16" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="19"/>
       <c r="B16" s="30" t="s">
+        <v>782</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>530</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>781</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>530</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>780</v>
-      </c>
       <c r="F16" s="28" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
@@ -10627,7 +10638,7 @@
     <row r="17" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="19"/>
       <c r="B17" s="30" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>30</v>
@@ -10648,11 +10659,11 @@
       <c r="O17" s="22"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A18" s="38" t="s">
-        <v>784</v>
+      <c r="A18" s="31" t="s">
+        <v>785</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>30</v>
@@ -10661,7 +10672,7 @@
         <v>253</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="F18" s="42"/>
       <c r="G18" s="27"/>
@@ -10675,9 +10686,9 @@
       <c r="O18" s="22"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A19" s="38"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="39" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C19" s="40" t="s">
         <v>30</v>
@@ -10686,7 +10697,7 @@
         <v>363</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="F19" s="42"/>
       <c r="G19" s="27"/>
@@ -10700,7 +10711,7 @@
       <c r="O19" s="22"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A20" s="38"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="39"/>
       <c r="C20" s="43" t="s">
         <v>8</v>
@@ -10709,10 +10720,10 @@
         <v>656</v>
       </c>
       <c r="E20" s="45" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F20" s="45" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
@@ -10727,7 +10738,7 @@
     <row r="21" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="19"/>
       <c r="B21" s="30" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>30</v>
@@ -10751,10 +10762,10 @@
     </row>
     <row r="22" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="19" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>30</v>
@@ -10763,7 +10774,7 @@
         <v>363</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
@@ -10778,17 +10789,17 @@
     </row>
     <row r="23" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="19"/>
-      <c r="B23" s="31" t="s">
-        <v>794</v>
-      </c>
-      <c r="C23" s="32" t="s">
+      <c r="B23" s="32" t="s">
+        <v>795</v>
+      </c>
+      <c r="C23" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="E23" s="33" t="s">
-        <v>795</v>
+      <c r="E23" s="34" t="s">
+        <v>796</v>
       </c>
       <c r="F23" s="47"/>
       <c r="G23" s="27"/>
@@ -10803,20 +10814,20 @@
     </row>
     <row r="24" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="19"/>
-      <c r="B24" s="31" t="s">
-        <v>796</v>
-      </c>
-      <c r="C24" s="32" t="s">
+      <c r="B24" s="32" t="s">
+        <v>797</v>
+      </c>
+      <c r="C24" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E24" s="33" t="s">
-        <v>797</v>
+      <c r="E24" s="34" t="s">
+        <v>798</v>
       </c>
       <c r="F24" s="47" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
@@ -10830,20 +10841,20 @@
     </row>
     <row r="25" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="19"/>
-      <c r="B25" s="31" t="s">
-        <v>799</v>
-      </c>
-      <c r="C25" s="32" t="s">
+      <c r="B25" s="32" t="s">
+        <v>800</v>
+      </c>
+      <c r="C25" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="34" t="s">
         <v>707</v>
       </c>
-      <c r="E25" s="33" t="s">
-        <v>800</v>
+      <c r="E25" s="34" t="s">
+        <v>801</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
@@ -10881,7 +10892,7 @@
     <row r="27" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A27" s="19"/>
       <c r="B27" s="30" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>30</v>
@@ -10890,10 +10901,10 @@
         <v>707</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
@@ -10908,19 +10919,19 @@
     <row r="28" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="19"/>
       <c r="B28" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C28" s="32" t="s">
+        <v>806</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E28" s="33" t="s">
-        <v>806</v>
+      <c r="E28" s="34" t="s">
+        <v>807</v>
       </c>
       <c r="F28" s="47" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
@@ -10935,19 +10946,19 @@
     <row r="29" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A29" s="19"/>
       <c r="B29" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C29" s="32" t="s">
+        <v>809</v>
+      </c>
+      <c r="C29" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E29" s="33" t="s">
-        <v>767</v>
+      <c r="E29" s="34" t="s">
+        <v>768</v>
       </c>
       <c r="F29" s="47" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
@@ -10962,19 +10973,19 @@
     <row r="30" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A30" s="19"/>
       <c r="B30" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C30" s="32" t="s">
+        <v>811</v>
+      </c>
+      <c r="C30" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
@@ -10989,19 +11000,19 @@
     <row r="31" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="19"/>
       <c r="B31" s="30" t="s">
-        <v>813</v>
-      </c>
-      <c r="C31" s="32" t="s">
+        <v>814</v>
+      </c>
+      <c r="C31" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
@@ -11016,19 +11027,19 @@
     <row r="32" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A32" s="19"/>
       <c r="B32" s="30" t="s">
-        <v>816</v>
-      </c>
-      <c r="C32" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="C32" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E32" s="33" t="s">
-        <v>817</v>
+      <c r="E32" s="34" t="s">
+        <v>818</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
@@ -11043,19 +11054,19 @@
     <row r="33" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="19"/>
       <c r="B33" s="30" t="s">
-        <v>819</v>
-      </c>
-      <c r="C33" s="32" t="s">
+        <v>820</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E33" s="33" t="s">
-        <v>820</v>
+      <c r="E33" s="34" t="s">
+        <v>821</v>
       </c>
       <c r="F33" s="47" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="27"/>
@@ -11070,19 +11081,19 @@
     <row r="34" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A34" s="19"/>
       <c r="B34" s="30" t="s">
-        <v>822</v>
-      </c>
-      <c r="C34" s="32" t="s">
+        <v>823</v>
+      </c>
+      <c r="C34" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
@@ -11097,17 +11108,17 @@
     <row r="35" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="19"/>
       <c r="B35" s="30"/>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="36" t="s">
         <v>656</v>
       </c>
       <c r="E35" s="48" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F35" s="49" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
@@ -11122,19 +11133,19 @@
     <row r="36" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="19"/>
       <c r="B36" s="30" t="s">
-        <v>825</v>
-      </c>
-      <c r="C36" s="32" t="s">
+        <v>826</v>
+      </c>
+      <c r="C36" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
@@ -11149,7 +11160,7 @@
     <row r="37" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A37" s="19"/>
       <c r="B37" s="30" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>30</v>
@@ -11158,7 +11169,7 @@
         <v>363</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
@@ -11173,17 +11184,17 @@
     </row>
     <row r="38" s="1" customFormat="1" ht="39" customHeight="1" spans="1:15">
       <c r="A38" s="19"/>
-      <c r="B38" s="31" t="s">
-        <v>829</v>
-      </c>
-      <c r="C38" s="32" t="s">
+      <c r="B38" s="32" t="s">
+        <v>830</v>
+      </c>
+      <c r="C38" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="34" t="s">
         <v>253</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="F38" s="47"/>
       <c r="G38" s="27"/>
@@ -11198,22 +11209,22 @@
     </row>
     <row r="39" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
       <c r="A39" s="19" t="s">
-        <v>831</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>796</v>
-      </c>
-      <c r="C39" s="32" t="s">
+        <v>832</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>797</v>
+      </c>
+      <c r="C39" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E39" s="33" t="s">
-        <v>832</v>
+      <c r="E39" s="34" t="s">
+        <v>833</v>
       </c>
       <c r="F39" s="47" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
@@ -11226,20 +11237,20 @@
       <c r="O39" s="22"/>
     </row>
     <row r="40" s="1" customFormat="1" ht="31" customHeight="1" spans="2:15">
-      <c r="B40" s="31" t="s">
-        <v>799</v>
-      </c>
-      <c r="C40" s="32" t="s">
+      <c r="B40" s="32" t="s">
+        <v>800</v>
+      </c>
+      <c r="C40" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="34" t="s">
         <v>707</v>
       </c>
-      <c r="E40" s="33" t="s">
-        <v>800</v>
+      <c r="E40" s="34" t="s">
+        <v>801</v>
       </c>
       <c r="F40" s="47" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -11253,17 +11264,17 @@
     </row>
     <row r="41" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A41" s="19"/>
-      <c r="B41" s="31" t="s">
-        <v>834</v>
-      </c>
-      <c r="C41" s="32" t="s">
+      <c r="B41" s="32" t="s">
+        <v>835</v>
+      </c>
+      <c r="C41" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="34" t="s">
         <v>363</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F41" s="47"/>
       <c r="G41" s="27"/>
@@ -11278,17 +11289,17 @@
     </row>
     <row r="42" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A42" s="19"/>
-      <c r="B42" s="31" t="s">
-        <v>836</v>
-      </c>
-      <c r="C42" s="32" t="s">
+      <c r="B42" s="32" t="s">
+        <v>837</v>
+      </c>
+      <c r="C42" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="34" t="s">
         <v>363</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="F42" s="47"/>
       <c r="G42" s="27"/>
@@ -11304,19 +11315,19 @@
     <row r="43" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A43" s="19"/>
       <c r="B43" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C43" s="32" t="s">
+        <v>806</v>
+      </c>
+      <c r="C43" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E43" s="33" t="s">
-        <v>838</v>
+      <c r="E43" s="34" t="s">
+        <v>839</v>
       </c>
       <c r="F43" s="47" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
@@ -11331,19 +11342,19 @@
     <row r="44" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A44" s="19"/>
       <c r="B44" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C44" s="32" t="s">
+        <v>809</v>
+      </c>
+      <c r="C44" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E44" s="33" t="s">
-        <v>839</v>
+      <c r="E44" s="34" t="s">
+        <v>840</v>
       </c>
       <c r="F44" s="47" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
@@ -11358,19 +11369,19 @@
     <row r="45" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A45" s="19"/>
       <c r="B45" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C45" s="32" t="s">
+        <v>811</v>
+      </c>
+      <c r="C45" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F45" s="27" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="G45" s="27"/>
       <c r="H45" s="27"/>
@@ -11385,19 +11396,19 @@
     <row r="46" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A46" s="19"/>
       <c r="B46" s="30" t="s">
-        <v>813</v>
-      </c>
-      <c r="C46" s="32" t="s">
+        <v>814</v>
+      </c>
+      <c r="C46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="33" t="s">
+      <c r="D46" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
@@ -11412,19 +11423,19 @@
     <row r="47" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A47" s="19"/>
       <c r="B47" s="30" t="s">
-        <v>816</v>
-      </c>
-      <c r="C47" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E47" s="33" t="s">
-        <v>843</v>
+      <c r="E47" s="34" t="s">
+        <v>844</v>
       </c>
       <c r="F47" s="47" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
@@ -11439,19 +11450,19 @@
     <row r="48" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A48" s="19"/>
       <c r="B48" s="30" t="s">
-        <v>819</v>
-      </c>
-      <c r="C48" s="32" t="s">
+        <v>820</v>
+      </c>
+      <c r="C48" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E48" s="33" t="s">
-        <v>844</v>
+      <c r="E48" s="34" t="s">
+        <v>845</v>
       </c>
       <c r="F48" s="47" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
@@ -11466,19 +11477,19 @@
     <row r="49" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A49" s="19"/>
       <c r="B49" s="30" t="s">
-        <v>822</v>
-      </c>
-      <c r="C49" s="32" t="s">
+        <v>823</v>
+      </c>
+      <c r="C49" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F49" s="27" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>
@@ -11493,17 +11504,17 @@
     <row r="50" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A50" s="19"/>
       <c r="B50" s="30"/>
-      <c r="C50" s="34" t="s">
+      <c r="C50" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="36" t="s">
         <v>656</v>
       </c>
       <c r="E50" s="48" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F50" s="49" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
@@ -11518,19 +11529,19 @@
     <row r="51" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A51" s="19"/>
       <c r="B51" s="30" t="s">
-        <v>825</v>
-      </c>
-      <c r="C51" s="32" t="s">
+        <v>826</v>
+      </c>
+      <c r="C51" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="33" t="s">
+      <c r="D51" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="F51" s="27" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="G51" s="27"/>
       <c r="H51" s="27"/>
@@ -11545,7 +11556,7 @@
     <row r="52" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A52" s="19"/>
       <c r="B52" s="30" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C52" s="26" t="s">
         <v>30</v>
@@ -11554,7 +11565,7 @@
         <v>363</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
@@ -11569,17 +11580,17 @@
     </row>
     <row r="53" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A53" s="19"/>
-      <c r="B53" s="31" t="s">
-        <v>829</v>
-      </c>
-      <c r="C53" s="32" t="s">
+      <c r="B53" s="32" t="s">
+        <v>830</v>
+      </c>
+      <c r="C53" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="33" t="s">
+      <c r="D53" s="34" t="s">
         <v>253</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
@@ -11594,7 +11605,7 @@
     </row>
     <row r="54" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B54" s="30" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>30</v>
@@ -11616,10 +11627,10 @@
     </row>
     <row r="55" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A55" s="19" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>30</v>
@@ -11628,10 +11639,10 @@
         <v>707</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="F55" s="27" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="G55" s="27"/>
       <c r="H55" s="27"/>
@@ -11644,9 +11655,11 @@
       <c r="O55" s="22"/>
     </row>
     <row r="56" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A56" s="19"/>
+      <c r="A56" s="31" t="s">
+        <v>853</v>
+      </c>
       <c r="B56" s="30" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>30</v>
@@ -11655,10 +11668,10 @@
         <v>576</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="F56" s="27" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="G56" s="27"/>
       <c r="H56" s="27"/>
@@ -11673,19 +11686,19 @@
     <row r="57" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A57" s="19"/>
       <c r="B57" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C57" s="32" t="s">
+        <v>806</v>
+      </c>
+      <c r="C57" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="33" t="s">
+      <c r="D57" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E57" s="33" t="s">
-        <v>855</v>
+      <c r="E57" s="34" t="s">
+        <v>857</v>
       </c>
       <c r="F57" s="47" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
@@ -11700,19 +11713,19 @@
     <row r="58" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A58" s="19"/>
       <c r="B58" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C58" s="32" t="s">
+        <v>809</v>
+      </c>
+      <c r="C58" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="D58" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E58" s="33" t="s">
-        <v>856</v>
+      <c r="E58" s="34" t="s">
+        <v>858</v>
       </c>
       <c r="F58" s="47" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="G58" s="27"/>
       <c r="H58" s="27"/>
@@ -11727,7 +11740,7 @@
     <row r="59" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A59" s="19"/>
       <c r="B59" s="30" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C59" s="26" t="s">
         <v>30</v>
@@ -11736,7 +11749,7 @@
         <v>363</v>
       </c>
       <c r="E59" s="47" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="F59" s="47"/>
       <c r="G59" s="27"/>
@@ -11752,19 +11765,19 @@
     <row r="60" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A60" s="19"/>
       <c r="B60" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C60" s="32" t="s">
+        <v>806</v>
+      </c>
+      <c r="C60" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E60" s="33" t="s">
-        <v>860</v>
+      <c r="E60" s="34" t="s">
+        <v>862</v>
       </c>
       <c r="F60" s="47" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G60" s="27"/>
       <c r="H60" s="27"/>
@@ -11779,19 +11792,19 @@
     <row r="61" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A61" s="19"/>
       <c r="B61" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C61" s="32" t="s">
+        <v>809</v>
+      </c>
+      <c r="C61" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="33" t="s">
+      <c r="D61" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E61" s="33" t="s">
-        <v>861</v>
+      <c r="E61" s="34" t="s">
+        <v>863</v>
       </c>
       <c r="F61" s="47" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="G61" s="27"/>
       <c r="H61" s="27"/>
@@ -11806,19 +11819,19 @@
     <row r="62" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A62" s="19"/>
       <c r="B62" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C62" s="32" t="s">
+        <v>811</v>
+      </c>
+      <c r="C62" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E62" s="28" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="F62" s="27" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="G62" s="27"/>
       <c r="H62" s="27"/>
@@ -11833,19 +11846,19 @@
     <row r="63" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A63" s="19"/>
       <c r="B63" s="30" t="s">
-        <v>813</v>
-      </c>
-      <c r="C63" s="32" t="s">
+        <v>814</v>
+      </c>
+      <c r="C63" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D63" s="33" t="s">
+      <c r="D63" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="F63" s="27" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="G63" s="27"/>
       <c r="H63" s="27"/>
@@ -11860,19 +11873,19 @@
     <row r="64" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A64" s="19"/>
       <c r="B64" s="30" t="s">
-        <v>816</v>
-      </c>
-      <c r="C64" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="C64" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D64" s="33" t="s">
+      <c r="D64" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E64" s="33" t="s">
-        <v>865</v>
+      <c r="E64" s="34" t="s">
+        <v>867</v>
       </c>
       <c r="F64" s="47" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="27"/>
@@ -11887,19 +11900,19 @@
     <row r="65" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A65" s="19"/>
       <c r="B65" s="30" t="s">
-        <v>819</v>
-      </c>
-      <c r="C65" s="32" t="s">
+        <v>820</v>
+      </c>
+      <c r="C65" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="33" t="s">
+      <c r="D65" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E65" s="33" t="s">
-        <v>866</v>
+      <c r="E65" s="34" t="s">
+        <v>868</v>
       </c>
       <c r="F65" s="47" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G65" s="27"/>
       <c r="H65" s="27"/>
@@ -11914,7 +11927,7 @@
     <row r="66" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A66" s="19"/>
       <c r="B66" s="30" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="C66" s="26" t="s">
         <v>30</v>
@@ -11923,7 +11936,7 @@
         <v>363</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="F66" s="27"/>
       <c r="G66" s="27"/>
@@ -11939,19 +11952,19 @@
     <row r="67" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A67" s="19"/>
       <c r="B67" s="30" t="s">
-        <v>816</v>
-      </c>
-      <c r="C67" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="C67" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="33" t="s">
+      <c r="D67" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E67" s="33" t="s">
-        <v>870</v>
+      <c r="E67" s="34" t="s">
+        <v>872</v>
       </c>
       <c r="F67" s="47" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G67" s="27"/>
       <c r="H67" s="27"/>
@@ -11966,19 +11979,19 @@
     <row r="68" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A68" s="19"/>
       <c r="B68" s="30" t="s">
-        <v>819</v>
-      </c>
-      <c r="C68" s="32" t="s">
+        <v>820</v>
+      </c>
+      <c r="C68" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D68" s="33" t="s">
+      <c r="D68" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E68" s="33" t="s">
-        <v>871</v>
+      <c r="E68" s="34" t="s">
+        <v>873</v>
       </c>
       <c r="F68" s="47" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="G68" s="27"/>
       <c r="H68" s="27"/>
@@ -11993,19 +12006,19 @@
     <row r="69" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A69" s="19"/>
       <c r="B69" s="30" t="s">
-        <v>822</v>
-      </c>
-      <c r="C69" s="32" t="s">
+        <v>823</v>
+      </c>
+      <c r="C69" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="33" t="s">
+      <c r="D69" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="F69" s="27" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="G69" s="27"/>
       <c r="H69" s="27"/>
@@ -12020,17 +12033,17 @@
     <row r="70" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A70" s="19"/>
       <c r="B70" s="30"/>
-      <c r="C70" s="34" t="s">
+      <c r="C70" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D70" s="35" t="s">
+      <c r="D70" s="36" t="s">
         <v>656</v>
       </c>
       <c r="E70" s="48" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F70" s="49" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="G70" s="27"/>
       <c r="H70" s="27"/>
@@ -12045,19 +12058,19 @@
     <row r="71" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A71" s="19"/>
       <c r="B71" s="30" t="s">
-        <v>825</v>
-      </c>
-      <c r="C71" s="32" t="s">
+        <v>826</v>
+      </c>
+      <c r="C71" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D71" s="33" t="s">
+      <c r="D71" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="F71" s="27" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="G71" s="27"/>
       <c r="H71" s="27"/>
@@ -12072,7 +12085,7 @@
     <row r="72" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A72" s="19"/>
       <c r="B72" s="30" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C72" s="26" t="s">
         <v>30</v>
@@ -12081,7 +12094,7 @@
         <v>363</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="F72" s="27"/>
       <c r="G72" s="27"/>
@@ -12097,7 +12110,7 @@
     <row r="73" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A73" s="19"/>
       <c r="B73" s="30" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="C73" s="26" t="s">
         <v>30</v>
@@ -12106,7 +12119,7 @@
         <v>253</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="F73" s="27"/>
       <c r="G73" s="27"/>
@@ -12121,16 +12134,16 @@
     </row>
     <row r="74" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A74" s="19"/>
-      <c r="B74" s="31" t="s">
-        <v>879</v>
-      </c>
-      <c r="C74" s="32" t="s">
+      <c r="B74" s="32" t="s">
+        <v>881</v>
+      </c>
+      <c r="C74" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D74" s="33" t="s">
+      <c r="D74" s="34" t="s">
         <v>620</v>
       </c>
-      <c r="E74" s="33"/>
+      <c r="E74" s="34"/>
       <c r="F74" s="47"/>
       <c r="G74" s="27"/>
       <c r="H74" s="27"/>
@@ -12144,10 +12157,10 @@
     </row>
     <row r="75" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A75" s="19" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>30</v>
@@ -12156,10 +12169,10 @@
         <v>707</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="F75" s="27" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="G75" s="27"/>
       <c r="H75" s="27"/>
@@ -12174,7 +12187,7 @@
     <row r="76" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A76" s="19"/>
       <c r="B76" s="30" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C76" s="26" t="s">
         <v>30</v>
@@ -12183,7 +12196,7 @@
         <v>363</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="F76" s="27"/>
       <c r="G76" s="27"/>
@@ -12199,19 +12212,19 @@
     <row r="77" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A77" s="19"/>
       <c r="B77" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C77" s="32" t="s">
+        <v>806</v>
+      </c>
+      <c r="C77" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D77" s="33" t="s">
+      <c r="D77" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E77" s="33" t="s">
-        <v>881</v>
+      <c r="E77" s="34" t="s">
+        <v>883</v>
       </c>
       <c r="F77" s="47" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G77" s="27"/>
       <c r="H77" s="27"/>
@@ -12226,19 +12239,19 @@
     <row r="78" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A78" s="19"/>
       <c r="B78" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C78" s="32" t="s">
+        <v>809</v>
+      </c>
+      <c r="C78" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D78" s="33" t="s">
+      <c r="D78" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E78" s="33" t="s">
-        <v>882</v>
+      <c r="E78" s="34" t="s">
+        <v>884</v>
       </c>
       <c r="F78" s="47" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="G78" s="27"/>
       <c r="H78" s="27"/>
@@ -12253,7 +12266,7 @@
     <row r="79" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A79" s="19"/>
       <c r="B79" s="30" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="C79" s="26" t="s">
         <v>30</v>
@@ -12262,7 +12275,7 @@
         <v>363</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="27"/>
@@ -12278,19 +12291,19 @@
     <row r="80" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A80" s="19"/>
       <c r="B80" s="30" t="s">
-        <v>816</v>
-      </c>
-      <c r="C80" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="C80" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="33" t="s">
+      <c r="D80" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E80" s="33" t="s">
-        <v>886</v>
+      <c r="E80" s="34" t="s">
+        <v>888</v>
       </c>
       <c r="F80" s="47" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -12305,19 +12318,19 @@
     <row r="81" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A81" s="19"/>
       <c r="B81" s="30" t="s">
-        <v>819</v>
-      </c>
-      <c r="C81" s="32" t="s">
+        <v>820</v>
+      </c>
+      <c r="C81" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="33" t="s">
+      <c r="D81" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E81" s="33" t="s">
-        <v>887</v>
+      <c r="E81" s="34" t="s">
+        <v>889</v>
       </c>
       <c r="F81" s="47" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="G81" s="27"/>
       <c r="H81" s="27"/>
@@ -12332,7 +12345,7 @@
     <row r="82" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A82" s="19"/>
       <c r="B82" s="30" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C82" s="26" t="s">
         <v>30</v>
@@ -12341,7 +12354,7 @@
         <v>363</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="F82" s="27"/>
       <c r="G82" s="27"/>
@@ -12357,7 +12370,7 @@
     <row r="83" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A83" s="19"/>
       <c r="B83" s="30" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>30</v>
@@ -12366,7 +12379,7 @@
         <v>363</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="F83" s="27"/>
       <c r="G83" s="27"/>
@@ -12380,9 +12393,11 @@
       <c r="O83" s="22"/>
     </row>
     <row r="84" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A84" s="19"/>
+      <c r="A84" s="31" t="s">
+        <v>893</v>
+      </c>
       <c r="B84" s="30" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="C84" s="26" t="s">
         <v>30</v>
@@ -12391,7 +12406,7 @@
         <v>253</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -12406,16 +12421,16 @@
     </row>
     <row r="85" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A85" s="19"/>
-      <c r="B85" s="31" t="s">
-        <v>879</v>
-      </c>
-      <c r="C85" s="32" t="s">
+      <c r="B85" s="32" t="s">
+        <v>881</v>
+      </c>
+      <c r="C85" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="33" t="s">
+      <c r="D85" s="34" t="s">
         <v>620</v>
       </c>
-      <c r="E85" s="33"/>
+      <c r="E85" s="34"/>
       <c r="F85" s="47"/>
       <c r="G85" s="27"/>
       <c r="H85" s="27"/>
@@ -12429,10 +12444,10 @@
     </row>
     <row r="86" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
       <c r="A86" s="19" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C86" s="26" t="s">
         <v>30</v>
@@ -12441,7 +12456,7 @@
         <v>363</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F86" s="47"/>
       <c r="G86" s="27"/>
@@ -12456,20 +12471,20 @@
     </row>
     <row r="87" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A87" s="19"/>
-      <c r="B87" s="31" t="s">
-        <v>799</v>
-      </c>
-      <c r="C87" s="32" t="s">
+      <c r="B87" s="32" t="s">
+        <v>800</v>
+      </c>
+      <c r="C87" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="33" t="s">
+      <c r="D87" s="34" t="s">
         <v>707</v>
       </c>
-      <c r="E87" s="33" t="s">
-        <v>800</v>
+      <c r="E87" s="34" t="s">
+        <v>801</v>
       </c>
       <c r="F87" s="47" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="G87" s="27"/>
       <c r="H87" s="27"/>
@@ -12483,17 +12498,17 @@
     </row>
     <row r="88" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A88" s="19"/>
-      <c r="B88" s="31" t="s">
-        <v>834</v>
-      </c>
-      <c r="C88" s="32" t="s">
+      <c r="B88" s="32" t="s">
+        <v>835</v>
+      </c>
+      <c r="C88" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D88" s="33" t="s">
+      <c r="D88" s="34" t="s">
         <v>363</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F88" s="47"/>
       <c r="G88" s="27"/>
@@ -12508,17 +12523,17 @@
     </row>
     <row r="89" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A89" s="19"/>
-      <c r="B89" s="31" t="s">
-        <v>836</v>
-      </c>
-      <c r="C89" s="32" t="s">
+      <c r="B89" s="32" t="s">
+        <v>837</v>
+      </c>
+      <c r="C89" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D89" s="33" t="s">
+      <c r="D89" s="34" t="s">
         <v>363</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="F89" s="47"/>
       <c r="G89" s="27"/>
@@ -12534,19 +12549,19 @@
     <row r="90" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A90" s="19"/>
       <c r="B90" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="C90" s="32" t="s">
+        <v>806</v>
+      </c>
+      <c r="C90" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D90" s="33" t="s">
+      <c r="D90" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E90" s="33" t="s">
-        <v>838</v>
+      <c r="E90" s="34" t="s">
+        <v>839</v>
       </c>
       <c r="F90" s="47" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
@@ -12561,19 +12576,19 @@
     <row r="91" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A91" s="19"/>
       <c r="B91" s="30" t="s">
-        <v>808</v>
-      </c>
-      <c r="C91" s="32" t="s">
+        <v>809</v>
+      </c>
+      <c r="C91" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="33" t="s">
+      <c r="D91" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E91" s="33" t="s">
-        <v>839</v>
+      <c r="E91" s="34" t="s">
+        <v>840</v>
       </c>
       <c r="F91" s="47" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="G91" s="27"/>
       <c r="H91" s="27"/>
@@ -12588,19 +12603,19 @@
     <row r="92" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A92" s="19"/>
       <c r="B92" s="30" t="s">
-        <v>810</v>
-      </c>
-      <c r="C92" s="32" t="s">
+        <v>811</v>
+      </c>
+      <c r="C92" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D92" s="33" t="s">
+      <c r="D92" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E92" s="28" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F92" s="27" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="G92" s="27"/>
       <c r="H92" s="27"/>
@@ -12615,19 +12630,19 @@
     <row r="93" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A93" s="19"/>
       <c r="B93" s="30" t="s">
-        <v>813</v>
-      </c>
-      <c r="C93" s="32" t="s">
+        <v>814</v>
+      </c>
+      <c r="C93" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D93" s="33" t="s">
+      <c r="D93" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="F93" s="27" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="G93" s="27"/>
       <c r="H93" s="27"/>
@@ -12642,19 +12657,19 @@
     <row r="94" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A94" s="19"/>
       <c r="B94" s="30" t="s">
-        <v>816</v>
-      </c>
-      <c r="C94" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="C94" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D94" s="33" t="s">
+      <c r="D94" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="E94" s="33" t="s">
-        <v>843</v>
+      <c r="E94" s="34" t="s">
+        <v>844</v>
       </c>
       <c r="F94" s="47" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G94" s="27"/>
       <c r="H94" s="27"/>
@@ -12669,19 +12684,19 @@
     <row r="95" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A95" s="19"/>
       <c r="B95" s="30" t="s">
-        <v>819</v>
-      </c>
-      <c r="C95" s="32" t="s">
+        <v>820</v>
+      </c>
+      <c r="C95" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D95" s="33" t="s">
+      <c r="D95" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="E95" s="33" t="s">
-        <v>844</v>
+      <c r="E95" s="34" t="s">
+        <v>845</v>
       </c>
       <c r="F95" s="47" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="G95" s="27"/>
       <c r="H95" s="27"/>
@@ -12696,19 +12711,19 @@
     <row r="96" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A96" s="19"/>
       <c r="B96" s="30" t="s">
-        <v>822</v>
-      </c>
-      <c r="C96" s="32" t="s">
+        <v>823</v>
+      </c>
+      <c r="C96" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D96" s="33" t="s">
+      <c r="D96" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E96" s="28" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F96" s="27" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="G96" s="27"/>
       <c r="H96" s="27"/>
@@ -12723,17 +12738,17 @@
     <row r="97" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A97" s="19"/>
       <c r="B97" s="30"/>
-      <c r="C97" s="34" t="s">
+      <c r="C97" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D97" s="35" t="s">
+      <c r="D97" s="36" t="s">
         <v>656</v>
       </c>
       <c r="E97" s="48" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F97" s="49" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="G97" s="27"/>
       <c r="H97" s="27"/>
@@ -12748,19 +12763,19 @@
     <row r="98" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A98" s="19"/>
       <c r="B98" s="30" t="s">
-        <v>825</v>
-      </c>
-      <c r="C98" s="32" t="s">
+        <v>826</v>
+      </c>
+      <c r="C98" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D98" s="33" t="s">
+      <c r="D98" s="34" t="s">
         <v>707</v>
       </c>
       <c r="E98" s="28" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="F98" s="27" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="G98" s="27"/>
       <c r="H98" s="27"/>
@@ -12775,7 +12790,7 @@
     <row r="99" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A99" s="19"/>
       <c r="B99" s="30" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C99" s="26" t="s">
         <v>30</v>
@@ -12784,7 +12799,7 @@
         <v>363</v>
       </c>
       <c r="E99" s="27" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="F99" s="27"/>
       <c r="G99" s="27"/>
@@ -12798,18 +12813,20 @@
       <c r="O99" s="22"/>
     </row>
     <row r="100" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A100" s="19"/>
-      <c r="B100" s="31" t="s">
-        <v>829</v>
-      </c>
-      <c r="C100" s="32" t="s">
+      <c r="A100" s="31" t="s">
+        <v>893</v>
+      </c>
+      <c r="B100" s="32" t="s">
+        <v>830</v>
+      </c>
+      <c r="C100" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D100" s="33" t="s">
+      <c r="D100" s="34" t="s">
         <v>253</v>
       </c>
       <c r="E100" s="27" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="F100" s="27"/>
       <c r="G100" s="27"/>
@@ -12824,7 +12841,7 @@
     </row>
     <row r="101" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B101" s="30" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="C101" s="26" t="s">
         <v>30</v>
@@ -12846,22 +12863,22 @@
     </row>
     <row r="102" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A102" s="19" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>851</v>
-      </c>
-      <c r="C102" s="32" t="s">
+        <v>852</v>
+      </c>
+      <c r="C102" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D102" s="33" t="s">
+      <c r="D102" s="34" t="s">
         <v>707</v>
       </c>
-      <c r="E102" s="33" t="s">
-        <v>764</v>
+      <c r="E102" s="34" t="s">
+        <v>765</v>
       </c>
       <c r="F102" s="47" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="G102" s="27"/>
       <c r="H102" s="27"/>
@@ -12876,7 +12893,7 @@
     <row r="103" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A103" s="19"/>
       <c r="B103" s="30" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="C103" s="26" t="s">
         <v>30</v>
@@ -12885,7 +12902,7 @@
         <v>600</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="F103" s="27"/>
       <c r="G103" s="27"/>
@@ -12901,7 +12918,7 @@
     <row r="104" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A104" s="19"/>
       <c r="B104" s="30" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>30</v>
@@ -12910,7 +12927,7 @@
         <v>253</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c r="F104" s="27"/>
       <c r="G104" s="27"/>
@@ -12926,7 +12943,7 @@
     <row r="105" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A105" s="19"/>
       <c r="B105" s="30" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>30</v>
@@ -12935,7 +12952,7 @@
         <v>363</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="F105" s="27"/>
       <c r="G105" s="27"/>
@@ -12951,7 +12968,7 @@
     <row r="106" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A106" s="19"/>
       <c r="B106" s="30" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="C106" s="26" t="s">
         <v>30</v>
@@ -12960,7 +12977,7 @@
         <v>363</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="F106" s="27"/>
       <c r="G106" s="27"/>
@@ -12974,9 +12991,11 @@
       <c r="O106" s="22"/>
     </row>
     <row r="107" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A107" s="19"/>
+      <c r="A107" s="31" t="s">
+        <v>893</v>
+      </c>
       <c r="B107" s="30" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="C107" s="26" t="s">
         <v>30</v>
@@ -12985,7 +13004,7 @@
         <v>253</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="F107" s="27"/>
       <c r="G107" s="27"/>
@@ -13001,7 +13020,7 @@
     <row r="108" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A108" s="19"/>
       <c r="B108" s="30" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C108" s="26" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Audit logs Script Updated
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-AddCategory.xlsx
+++ b/tests/artifact/script/UI-AddCategory.xlsx
@@ -10176,10 +10176,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O200"/>
+  <dimension ref="A1:O201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A9" sqref="$A9:$XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -10394,7 +10394,7 @@
       <c r="N7" s="23"/>
       <c r="O7" s="22"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="8" s="1" customFormat="1" ht="68" customHeight="1" spans="1:15">
       <c r="A8" s="31" t="s">
         <v>760</v>
       </c>
@@ -10422,24 +10422,12 @@
       <c r="O8" s="22"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A9" s="19" t="s">
-        <v>763</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>764</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>765</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>766</v>
-      </c>
+      <c r="A9" s="19"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
@@ -10451,21 +10439,23 @@
       <c r="O9" s="22"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A10" s="19"/>
-      <c r="B10" s="30" t="s">
-        <v>767</v>
-      </c>
-      <c r="C10" s="26" t="s">
+      <c r="A10" s="19" t="s">
+        <v>763</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>764</v>
+      </c>
+      <c r="C10" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>483</v>
+      <c r="D10" s="34" t="s">
+        <v>707</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>768</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>769</v>
+        <v>765</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>766</v>
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
@@ -10480,19 +10470,19 @@
     <row r="11" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A11" s="19"/>
       <c r="B11" s="30" t="s">
-        <v>770</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>471</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>771</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>772</v>
+        <v>767</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>483</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>768</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>769</v>
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
@@ -10506,18 +10496,20 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A12" s="19"/>
-      <c r="B12" s="30"/>
+      <c r="B12" s="30" t="s">
+        <v>770</v>
+      </c>
       <c r="C12" s="35" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
@@ -10535,14 +10527,14 @@
       <c r="C13" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="38" t="s">
-        <v>49</v>
+      <c r="D13" s="36" t="s">
+        <v>465</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>775</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>776</v>
+        <v>773</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>774</v>
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -10556,20 +10548,18 @@
     </row>
     <row r="14" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="19"/>
-      <c r="B14" s="30" t="s">
-        <v>777</v>
-      </c>
+      <c r="B14" s="30"/>
       <c r="C14" s="35" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>302</v>
+        <v>49</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>771</v>
-      </c>
-      <c r="F14" s="37" t="s">
-        <v>778</v>
+        <v>775</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>776</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -10584,19 +10574,19 @@
     <row r="15" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A15" s="19"/>
       <c r="B15" s="30" t="s">
-        <v>779</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>493</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>780</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>781</v>
+        <v>777</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>771</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>778</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -10611,19 +10601,19 @@
     <row r="16" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="19"/>
       <c r="B16" s="30" t="s">
-        <v>782</v>
-      </c>
-      <c r="C16" s="35" t="s">
+        <v>779</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="36" t="s">
-        <v>530</v>
-      </c>
-      <c r="E16" s="28" t="s">
+      <c r="D16" s="27" t="s">
+        <v>493</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>780</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>781</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>783</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
@@ -10638,16 +10628,20 @@
     <row r="17" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="19"/>
       <c r="B17" s="30" t="s">
-        <v>784</v>
-      </c>
-      <c r="C17" s="26" t="s">
+        <v>782</v>
+      </c>
+      <c r="C17" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
+      <c r="D17" s="36" t="s">
+        <v>530</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>781</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>783</v>
+      </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
       <c r="I17" s="27"/>
@@ -10659,22 +10653,18 @@
       <c r="O17" s="22"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A18" s="31" t="s">
-        <v>785</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>786</v>
-      </c>
-      <c r="C18" s="40" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="30" t="s">
+        <v>784</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="41" t="s">
-        <v>253</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>787</v>
-      </c>
-      <c r="F18" s="42"/>
+      <c r="D18" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
       <c r="I18" s="27"/>
@@ -10686,15 +10676,17 @@
       <c r="O18" s="22"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A19" s="31"/>
+      <c r="A19" s="31" t="s">
+        <v>785</v>
+      </c>
       <c r="B19" s="39" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C19" s="40" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>363</v>
+        <v>253</v>
       </c>
       <c r="E19" s="41" t="s">
         <v>787</v>
@@ -10712,19 +10704,19 @@
     </row>
     <row r="20" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A20" s="31"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>656</v>
-      </c>
-      <c r="E20" s="45" t="s">
-        <v>789</v>
-      </c>
-      <c r="F20" s="45" t="s">
-        <v>790</v>
-      </c>
+      <c r="B20" s="39" t="s">
+        <v>788</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>787</v>
+      </c>
+      <c r="F20" s="42"/>
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
@@ -10736,20 +10728,20 @@
       <c r="O20" s="22"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A21" s="19"/>
-      <c r="B21" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>715</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>759</v>
-      </c>
-      <c r="F21" s="46"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>656</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>789</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>790</v>
+      </c>
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
@@ -10761,22 +10753,20 @@
       <c r="O21" s="22"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A22" s="19" t="s">
-        <v>792</v>
-      </c>
+      <c r="A22" s="19"/>
       <c r="B22" s="30" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>794</v>
-      </c>
-      <c r="F22" s="27"/>
+        <v>715</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>759</v>
+      </c>
+      <c r="F22" s="46"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
@@ -10788,20 +10778,22 @@
       <c r="O22" s="22"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A23" s="19"/>
-      <c r="B23" s="32" t="s">
-        <v>795</v>
-      </c>
-      <c r="C23" s="33" t="s">
+      <c r="A23" s="19" t="s">
+        <v>792</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>793</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>796</v>
-      </c>
-      <c r="F23" s="47"/>
+      <c r="D23" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>794</v>
+      </c>
+      <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
@@ -10815,20 +10807,18 @@
     <row r="24" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="19"/>
       <c r="B24" s="32" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>471</v>
+        <v>253</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>798</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>799</v>
-      </c>
+        <v>796</v>
+      </c>
+      <c r="F24" s="47"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
@@ -10842,19 +10832,19 @@
     <row r="25" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="19"/>
       <c r="B25" s="32" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>707</v>
+        <v>471</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
@@ -10868,17 +10858,21 @@
     </row>
     <row r="26" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A26" s="19"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="32" t="s">
+        <v>800</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="27" t="s">
-        <v>715</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>759</v>
-      </c>
-      <c r="F26" s="27"/>
+      <c r="D26" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>801</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>802</v>
+      </c>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
       <c r="I26" s="27"/>
@@ -10891,21 +10885,17 @@
     </row>
     <row r="27" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A27" s="19"/>
-      <c r="B27" s="30" t="s">
-        <v>803</v>
-      </c>
+      <c r="B27" s="30"/>
       <c r="C27" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>804</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>805</v>
-      </c>
+        <v>759</v>
+      </c>
+      <c r="F27" s="27"/>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
@@ -10919,19 +10909,19 @@
     <row r="28" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="19"/>
       <c r="B28" s="30" t="s">
-        <v>806</v>
-      </c>
-      <c r="C28" s="33" t="s">
+        <v>803</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E28" s="34" t="s">
-        <v>807</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>808</v>
+      <c r="D28" s="27" t="s">
+        <v>707</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>804</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>805</v>
       </c>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
@@ -10946,19 +10936,19 @@
     <row r="29" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A29" s="19"/>
       <c r="B29" s="30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>768</v>
+        <v>807</v>
       </c>
       <c r="F29" s="47" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
@@ -10973,19 +10963,19 @@
     <row r="30" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A30" s="19"/>
       <c r="B30" s="30" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>812</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>813</v>
+        <v>471</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>768</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>810</v>
       </c>
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
@@ -11000,7 +10990,7 @@
     <row r="31" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="19"/>
       <c r="B31" s="30" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="C31" s="33" t="s">
         <v>30</v>
@@ -11009,10 +10999,10 @@
         <v>707</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
@@ -11027,19 +11017,19 @@
     <row r="32" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A32" s="19"/>
       <c r="B32" s="30" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="C32" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>818</v>
-      </c>
-      <c r="F32" s="47" t="s">
-        <v>819</v>
+        <v>707</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>815</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>816</v>
       </c>
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
@@ -11054,19 +11044,19 @@
     <row r="33" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="19"/>
       <c r="B33" s="30" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="F33" s="47" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="27"/>
@@ -11081,19 +11071,19 @@
     <row r="34" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A34" s="19"/>
       <c r="B34" s="30" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E34" s="28" t="s">
-        <v>824</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>825</v>
+        <v>471</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>821</v>
+      </c>
+      <c r="F34" s="47" t="s">
+        <v>822</v>
       </c>
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
@@ -11107,18 +11097,20 @@
     </row>
     <row r="35" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="19"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="36" t="s">
-        <v>656</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>789</v>
-      </c>
-      <c r="F35" s="49" t="s">
-        <v>790</v>
+      <c r="B35" s="30" t="s">
+        <v>823</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>824</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>825</v>
       </c>
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
@@ -11132,20 +11124,18 @@
     </row>
     <row r="36" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="19"/>
-      <c r="B36" s="30" t="s">
-        <v>826</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>827</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>778</v>
+      <c r="B36" s="30"/>
+      <c r="C36" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>789</v>
+      </c>
+      <c r="F36" s="49" t="s">
+        <v>790</v>
       </c>
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
@@ -11160,18 +11150,20 @@
     <row r="37" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A37" s="19"/>
       <c r="B37" s="30" t="s">
-        <v>828</v>
-      </c>
-      <c r="C37" s="26" t="s">
+        <v>826</v>
+      </c>
+      <c r="C37" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>829</v>
-      </c>
-      <c r="F37" s="27"/>
+      <c r="D37" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>827</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>778</v>
+      </c>
       <c r="G37" s="27"/>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
@@ -11182,21 +11174,21 @@
       <c r="N37" s="23"/>
       <c r="O37" s="22"/>
     </row>
-    <row r="38" s="1" customFormat="1" ht="39" customHeight="1" spans="1:15">
+    <row r="38" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A38" s="19"/>
-      <c r="B38" s="32" t="s">
-        <v>830</v>
-      </c>
-      <c r="C38" s="33" t="s">
+      <c r="B38" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="C38" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="34" t="s">
-        <v>253</v>
+      <c r="D38" s="27" t="s">
+        <v>363</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>831</v>
-      </c>
-      <c r="F38" s="47"/>
+        <v>829</v>
+      </c>
+      <c r="F38" s="27"/>
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
       <c r="I38" s="27"/>
@@ -11207,25 +11199,21 @@
       <c r="N38" s="23"/>
       <c r="O38" s="22"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
-      <c r="A39" s="19" t="s">
-        <v>832</v>
-      </c>
+    <row r="39" s="1" customFormat="1" ht="39" customHeight="1" spans="1:15">
+      <c r="A39" s="19"/>
       <c r="B39" s="32" t="s">
-        <v>797</v>
+        <v>830</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="E39" s="34" t="s">
-        <v>833</v>
-      </c>
-      <c r="F39" s="47" t="s">
-        <v>799</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>831</v>
+      </c>
+      <c r="F39" s="47"/>
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
       <c r="I39" s="27"/>
@@ -11236,21 +11224,24 @@
       <c r="N39" s="23"/>
       <c r="O39" s="22"/>
     </row>
-    <row r="40" s="1" customFormat="1" ht="31" customHeight="1" spans="2:15">
+    <row r="40" s="1" customFormat="1" ht="31" customHeight="1" spans="1:15">
+      <c r="A40" s="19" t="s">
+        <v>832</v>
+      </c>
       <c r="B40" s="32" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D40" s="34" t="s">
-        <v>707</v>
+        <v>471</v>
       </c>
       <c r="E40" s="34" t="s">
-        <v>801</v>
+        <v>833</v>
       </c>
       <c r="F40" s="47" t="s">
-        <v>834</v>
+        <v>799</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -11262,21 +11253,22 @@
       <c r="N40" s="23"/>
       <c r="O40" s="22"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A41" s="19"/>
+    <row r="41" s="1" customFormat="1" ht="31" customHeight="1" spans="2:15">
       <c r="B41" s="32" t="s">
-        <v>835</v>
+        <v>800</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E41" s="27" t="s">
-        <v>836</v>
-      </c>
-      <c r="F41" s="47"/>
+        <v>707</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>801</v>
+      </c>
+      <c r="F41" s="47" t="s">
+        <v>834</v>
+      </c>
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
       <c r="I41" s="27"/>
@@ -11290,7 +11282,7 @@
     <row r="42" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A42" s="19"/>
       <c r="B42" s="32" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>30</v>
@@ -11299,7 +11291,7 @@
         <v>363</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="F42" s="47"/>
       <c r="G42" s="27"/>
@@ -11314,21 +11306,19 @@
     </row>
     <row r="43" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A43" s="19"/>
-      <c r="B43" s="30" t="s">
-        <v>806</v>
+      <c r="B43" s="32" t="s">
+        <v>837</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E43" s="34" t="s">
-        <v>839</v>
-      </c>
-      <c r="F43" s="47" t="s">
-        <v>808</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>838</v>
+      </c>
+      <c r="F43" s="47"/>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
       <c r="I43" s="27"/>
@@ -11342,19 +11332,19 @@
     <row r="44" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A44" s="19"/>
       <c r="B44" s="30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F44" s="47" t="s">
-        <v>841</v>
+        <v>808</v>
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
@@ -11369,19 +11359,19 @@
     <row r="45" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A45" s="19"/>
       <c r="B45" s="30" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>842</v>
-      </c>
-      <c r="F45" s="27" t="s">
-        <v>813</v>
+        <v>471</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>840</v>
+      </c>
+      <c r="F45" s="47" t="s">
+        <v>841</v>
       </c>
       <c r="G45" s="27"/>
       <c r="H45" s="27"/>
@@ -11396,7 +11386,7 @@
     <row r="46" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A46" s="19"/>
       <c r="B46" s="30" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>30</v>
@@ -11405,10 +11395,10 @@
         <v>707</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
@@ -11423,19 +11413,19 @@
     <row r="47" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A47" s="19"/>
       <c r="B47" s="30" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E47" s="34" t="s">
-        <v>844</v>
-      </c>
-      <c r="F47" s="47" t="s">
-        <v>819</v>
+        <v>707</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>843</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>816</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
@@ -11450,19 +11440,19 @@
     <row r="48" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A48" s="19"/>
       <c r="B48" s="30" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F48" s="47" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
@@ -11477,19 +11467,19 @@
     <row r="49" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A49" s="19"/>
       <c r="B49" s="30" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>846</v>
-      </c>
-      <c r="F49" s="27" t="s">
-        <v>847</v>
+        <v>471</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>845</v>
+      </c>
+      <c r="F49" s="47" t="s">
+        <v>822</v>
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>
@@ -11503,18 +11493,20 @@
     </row>
     <row r="50" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A50" s="19"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="36" t="s">
-        <v>656</v>
-      </c>
-      <c r="E50" s="48" t="s">
-        <v>789</v>
-      </c>
-      <c r="F50" s="49" t="s">
-        <v>790</v>
+      <c r="B50" s="30" t="s">
+        <v>823</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>846</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>847</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
@@ -11528,20 +11520,18 @@
     </row>
     <row r="51" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A51" s="19"/>
-      <c r="B51" s="30" t="s">
-        <v>826</v>
-      </c>
-      <c r="C51" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E51" s="28" t="s">
-        <v>848</v>
-      </c>
-      <c r="F51" s="27" t="s">
-        <v>778</v>
+      <c r="B51" s="30"/>
+      <c r="C51" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="E51" s="48" t="s">
+        <v>789</v>
+      </c>
+      <c r="F51" s="49" t="s">
+        <v>790</v>
       </c>
       <c r="G51" s="27"/>
       <c r="H51" s="27"/>
@@ -11556,18 +11546,20 @@
     <row r="52" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A52" s="19"/>
       <c r="B52" s="30" t="s">
-        <v>828</v>
-      </c>
-      <c r="C52" s="26" t="s">
+        <v>826</v>
+      </c>
+      <c r="C52" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E52" s="27" t="s">
-        <v>829</v>
-      </c>
-      <c r="F52" s="27"/>
+      <c r="D52" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>848</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>778</v>
+      </c>
       <c r="G52" s="27"/>
       <c r="H52" s="27"/>
       <c r="I52" s="27"/>
@@ -11580,17 +11572,17 @@
     </row>
     <row r="53" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A53" s="19"/>
-      <c r="B53" s="32" t="s">
-        <v>830</v>
-      </c>
-      <c r="C53" s="33" t="s">
+      <c r="B53" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="C53" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="34" t="s">
-        <v>253</v>
+      <c r="D53" s="27" t="s">
+        <v>363</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>849</v>
+        <v>829</v>
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
@@ -11603,17 +11595,20 @@
       <c r="N53" s="23"/>
       <c r="O53" s="22"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B54" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="C54" s="26" t="s">
+    <row r="54" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A54" s="19"/>
+      <c r="B54" s="32" t="s">
+        <v>830</v>
+      </c>
+      <c r="C54" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="27" t="s">
-        <v>620</v>
-      </c>
-      <c r="E54" s="27"/>
+      <c r="D54" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>849</v>
+      </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
       <c r="H54" s="27"/>
@@ -11625,25 +11620,18 @@
       <c r="N54" s="23"/>
       <c r="O54" s="22"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A55" s="19" t="s">
-        <v>851</v>
-      </c>
+    <row r="55" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B55" s="30" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>707</v>
-      </c>
-      <c r="E55" s="27" t="s">
-        <v>765</v>
-      </c>
-      <c r="F55" s="27" t="s">
-        <v>802</v>
-      </c>
+        <v>620</v>
+      </c>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
       <c r="G55" s="27"/>
       <c r="H55" s="27"/>
       <c r="I55" s="27"/>
@@ -11655,23 +11643,23 @@
       <c r="O55" s="22"/>
     </row>
     <row r="56" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A56" s="31" t="s">
-        <v>853</v>
+      <c r="A56" s="19" t="s">
+        <v>851</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>576</v>
+        <v>707</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>855</v>
+        <v>765</v>
       </c>
       <c r="F56" s="27" t="s">
-        <v>856</v>
+        <v>802</v>
       </c>
       <c r="G56" s="27"/>
       <c r="H56" s="27"/>
@@ -11683,22 +11671,24 @@
       <c r="N56" s="23"/>
       <c r="O56" s="22"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A57" s="19"/>
+    <row r="57" s="1" customFormat="1" ht="46" customHeight="1" spans="1:15">
+      <c r="A57" s="31" t="s">
+        <v>853</v>
+      </c>
       <c r="B57" s="30" t="s">
-        <v>806</v>
-      </c>
-      <c r="C57" s="33" t="s">
+        <v>854</v>
+      </c>
+      <c r="C57" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>857</v>
-      </c>
-      <c r="F57" s="47" t="s">
-        <v>808</v>
+      <c r="D57" s="27" t="s">
+        <v>576</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>855</v>
+      </c>
+      <c r="F57" s="27" t="s">
+        <v>856</v>
       </c>
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
@@ -11713,19 +11703,19 @@
     <row r="58" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A58" s="19"/>
       <c r="B58" s="30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E58" s="34" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F58" s="47" t="s">
-        <v>859</v>
+        <v>808</v>
       </c>
       <c r="G58" s="27"/>
       <c r="H58" s="27"/>
@@ -11740,18 +11730,20 @@
     <row r="59" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A59" s="19"/>
       <c r="B59" s="30" t="s">
-        <v>860</v>
-      </c>
-      <c r="C59" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D59" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E59" s="47" t="s">
-        <v>861</v>
-      </c>
-      <c r="F59" s="47"/>
+        <v>809</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>858</v>
+      </c>
+      <c r="F59" s="47" t="s">
+        <v>859</v>
+      </c>
       <c r="G59" s="27"/>
       <c r="H59" s="27"/>
       <c r="I59" s="27"/>
@@ -11765,20 +11757,18 @@
     <row r="60" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A60" s="19"/>
       <c r="B60" s="30" t="s">
-        <v>806</v>
-      </c>
-      <c r="C60" s="33" t="s">
+        <v>860</v>
+      </c>
+      <c r="C60" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D60" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E60" s="34" t="s">
-        <v>862</v>
-      </c>
-      <c r="F60" s="47" t="s">
-        <v>808</v>
-      </c>
+      <c r="D60" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E60" s="47" t="s">
+        <v>861</v>
+      </c>
+      <c r="F60" s="47"/>
       <c r="G60" s="27"/>
       <c r="H60" s="27"/>
       <c r="I60" s="27"/>
@@ -11792,19 +11782,19 @@
     <row r="61" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A61" s="19"/>
       <c r="B61" s="30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D61" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E61" s="34" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F61" s="47" t="s">
-        <v>864</v>
+        <v>808</v>
       </c>
       <c r="G61" s="27"/>
       <c r="H61" s="27"/>
@@ -11819,19 +11809,19 @@
     <row r="62" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A62" s="19"/>
       <c r="B62" s="30" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E62" s="28" t="s">
-        <v>865</v>
-      </c>
-      <c r="F62" s="27" t="s">
-        <v>813</v>
+        <v>471</v>
+      </c>
+      <c r="E62" s="34" t="s">
+        <v>863</v>
+      </c>
+      <c r="F62" s="47" t="s">
+        <v>864</v>
       </c>
       <c r="G62" s="27"/>
       <c r="H62" s="27"/>
@@ -11846,7 +11836,7 @@
     <row r="63" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A63" s="19"/>
       <c r="B63" s="30" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="C63" s="33" t="s">
         <v>30</v>
@@ -11855,10 +11845,10 @@
         <v>707</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="F63" s="27" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="G63" s="27"/>
       <c r="H63" s="27"/>
@@ -11873,19 +11863,19 @@
     <row r="64" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A64" s="19"/>
       <c r="B64" s="30" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="C64" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E64" s="34" t="s">
-        <v>867</v>
-      </c>
-      <c r="F64" s="47" t="s">
-        <v>819</v>
+        <v>707</v>
+      </c>
+      <c r="E64" s="28" t="s">
+        <v>866</v>
+      </c>
+      <c r="F64" s="27" t="s">
+        <v>816</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="27"/>
@@ -11900,19 +11890,19 @@
     <row r="65" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A65" s="19"/>
       <c r="B65" s="30" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D65" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E65" s="34" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F65" s="47" t="s">
-        <v>869</v>
+        <v>819</v>
       </c>
       <c r="G65" s="27"/>
       <c r="H65" s="27"/>
@@ -11927,18 +11917,20 @@
     <row r="66" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A66" s="19"/>
       <c r="B66" s="30" t="s">
-        <v>870</v>
-      </c>
-      <c r="C66" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>871</v>
-      </c>
-      <c r="F66" s="27"/>
+        <v>820</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="E66" s="34" t="s">
+        <v>868</v>
+      </c>
+      <c r="F66" s="47" t="s">
+        <v>869</v>
+      </c>
       <c r="G66" s="27"/>
       <c r="H66" s="27"/>
       <c r="I66" s="27"/>
@@ -11952,20 +11944,18 @@
     <row r="67" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A67" s="19"/>
       <c r="B67" s="30" t="s">
-        <v>817</v>
-      </c>
-      <c r="C67" s="33" t="s">
+        <v>870</v>
+      </c>
+      <c r="C67" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E67" s="34" t="s">
-        <v>872</v>
-      </c>
-      <c r="F67" s="47" t="s">
-        <v>819</v>
-      </c>
+      <c r="D67" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E67" s="27" t="s">
+        <v>871</v>
+      </c>
+      <c r="F67" s="27"/>
       <c r="G67" s="27"/>
       <c r="H67" s="27"/>
       <c r="I67" s="27"/>
@@ -11979,19 +11969,19 @@
     <row r="68" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A68" s="19"/>
       <c r="B68" s="30" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E68" s="34" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F68" s="47" t="s">
-        <v>874</v>
+        <v>819</v>
       </c>
       <c r="G68" s="27"/>
       <c r="H68" s="27"/>
@@ -12006,19 +11996,19 @@
     <row r="69" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A69" s="19"/>
       <c r="B69" s="30" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E69" s="28" t="s">
-        <v>875</v>
-      </c>
-      <c r="F69" s="27" t="s">
-        <v>847</v>
+        <v>471</v>
+      </c>
+      <c r="E69" s="34" t="s">
+        <v>873</v>
+      </c>
+      <c r="F69" s="47" t="s">
+        <v>874</v>
       </c>
       <c r="G69" s="27"/>
       <c r="H69" s="27"/>
@@ -12032,18 +12022,20 @@
     </row>
     <row r="70" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A70" s="19"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="36" t="s">
-        <v>656</v>
-      </c>
-      <c r="E70" s="48" t="s">
-        <v>789</v>
-      </c>
-      <c r="F70" s="49" t="s">
-        <v>790</v>
+      <c r="B70" s="30" t="s">
+        <v>823</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>875</v>
+      </c>
+      <c r="F70" s="27" t="s">
+        <v>847</v>
       </c>
       <c r="G70" s="27"/>
       <c r="H70" s="27"/>
@@ -12057,20 +12049,18 @@
     </row>
     <row r="71" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A71" s="19"/>
-      <c r="B71" s="30" t="s">
-        <v>826</v>
-      </c>
-      <c r="C71" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E71" s="28" t="s">
-        <v>876</v>
-      </c>
-      <c r="F71" s="27" t="s">
-        <v>778</v>
+      <c r="B71" s="30"/>
+      <c r="C71" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="E71" s="48" t="s">
+        <v>789</v>
+      </c>
+      <c r="F71" s="49" t="s">
+        <v>790</v>
       </c>
       <c r="G71" s="27"/>
       <c r="H71" s="27"/>
@@ -12085,18 +12075,20 @@
     <row r="72" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A72" s="19"/>
       <c r="B72" s="30" t="s">
-        <v>877</v>
-      </c>
-      <c r="C72" s="26" t="s">
+        <v>826</v>
+      </c>
+      <c r="C72" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D72" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E72" s="27" t="s">
-        <v>878</v>
-      </c>
-      <c r="F72" s="27"/>
+      <c r="D72" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>876</v>
+      </c>
+      <c r="F72" s="27" t="s">
+        <v>778</v>
+      </c>
       <c r="G72" s="27"/>
       <c r="H72" s="27"/>
       <c r="I72" s="27"/>
@@ -12110,16 +12102,16 @@
     <row r="73" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A73" s="19"/>
       <c r="B73" s="30" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C73" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>253</v>
+        <v>363</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="F73" s="27"/>
       <c r="G73" s="27"/>
@@ -12134,17 +12126,19 @@
     </row>
     <row r="74" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A74" s="19"/>
-      <c r="B74" s="32" t="s">
-        <v>881</v>
-      </c>
-      <c r="C74" s="33" t="s">
+      <c r="B74" s="30" t="s">
+        <v>879</v>
+      </c>
+      <c r="C74" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D74" s="34" t="s">
-        <v>620</v>
-      </c>
-      <c r="E74" s="34"/>
-      <c r="F74" s="47"/>
+      <c r="D74" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E74" s="27" t="s">
+        <v>880</v>
+      </c>
+      <c r="F74" s="27"/>
       <c r="G74" s="27"/>
       <c r="H74" s="27"/>
       <c r="I74" s="27"/>
@@ -12156,24 +12150,18 @@
       <c r="O74" s="22"/>
     </row>
     <row r="75" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A75" s="19" t="s">
-        <v>882</v>
-      </c>
-      <c r="B75" s="30" t="s">
-        <v>852</v>
-      </c>
-      <c r="C75" s="26" t="s">
+      <c r="A75" s="19"/>
+      <c r="B75" s="32" t="s">
+        <v>881</v>
+      </c>
+      <c r="C75" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D75" s="27" t="s">
-        <v>707</v>
-      </c>
-      <c r="E75" s="27" t="s">
-        <v>765</v>
-      </c>
-      <c r="F75" s="27" t="s">
-        <v>802</v>
-      </c>
+      <c r="D75" s="34" t="s">
+        <v>620</v>
+      </c>
+      <c r="E75" s="34"/>
+      <c r="F75" s="47"/>
       <c r="G75" s="27"/>
       <c r="H75" s="27"/>
       <c r="I75" s="27"/>
@@ -12184,21 +12172,25 @@
       <c r="N75" s="23"/>
       <c r="O75" s="22"/>
     </row>
-    <row r="76" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A76" s="19"/>
+    <row r="76" s="1" customFormat="1" ht="41" customHeight="1" spans="1:15">
+      <c r="A76" s="19" t="s">
+        <v>882</v>
+      </c>
       <c r="B76" s="30" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="C76" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D76" s="27" t="s">
-        <v>363</v>
+        <v>707</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>855</v>
-      </c>
-      <c r="F76" s="27"/>
+        <v>765</v>
+      </c>
+      <c r="F76" s="27" t="s">
+        <v>802</v>
+      </c>
       <c r="G76" s="27"/>
       <c r="H76" s="27"/>
       <c r="I76" s="27"/>
@@ -12212,20 +12204,18 @@
     <row r="77" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A77" s="19"/>
       <c r="B77" s="30" t="s">
-        <v>806</v>
-      </c>
-      <c r="C77" s="33" t="s">
+        <v>854</v>
+      </c>
+      <c r="C77" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D77" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E77" s="34" t="s">
-        <v>883</v>
-      </c>
-      <c r="F77" s="47" t="s">
-        <v>808</v>
-      </c>
+      <c r="D77" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E77" s="27" t="s">
+        <v>855</v>
+      </c>
+      <c r="F77" s="27"/>
       <c r="G77" s="27"/>
       <c r="H77" s="27"/>
       <c r="I77" s="27"/>
@@ -12239,19 +12229,19 @@
     <row r="78" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A78" s="19"/>
       <c r="B78" s="30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D78" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E78" s="34" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F78" s="47" t="s">
-        <v>885</v>
+        <v>808</v>
       </c>
       <c r="G78" s="27"/>
       <c r="H78" s="27"/>
@@ -12266,18 +12256,20 @@
     <row r="79" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A79" s="19"/>
       <c r="B79" s="30" t="s">
-        <v>886</v>
-      </c>
-      <c r="C79" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D79" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E79" s="27" t="s">
-        <v>887</v>
-      </c>
-      <c r="F79" s="27"/>
+        <v>809</v>
+      </c>
+      <c r="C79" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="E79" s="34" t="s">
+        <v>884</v>
+      </c>
+      <c r="F79" s="47" t="s">
+        <v>885</v>
+      </c>
       <c r="G79" s="27"/>
       <c r="H79" s="27"/>
       <c r="I79" s="27"/>
@@ -12291,20 +12283,18 @@
     <row r="80" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A80" s="19"/>
       <c r="B80" s="30" t="s">
-        <v>817</v>
-      </c>
-      <c r="C80" s="33" t="s">
+        <v>886</v>
+      </c>
+      <c r="C80" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E80" s="34" t="s">
-        <v>888</v>
-      </c>
-      <c r="F80" s="47" t="s">
-        <v>819</v>
-      </c>
+      <c r="D80" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E80" s="27" t="s">
+        <v>887</v>
+      </c>
+      <c r="F80" s="27"/>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
       <c r="I80" s="27"/>
@@ -12318,19 +12308,19 @@
     <row r="81" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A81" s="19"/>
       <c r="B81" s="30" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D81" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E81" s="34" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="F81" s="47" t="s">
-        <v>890</v>
+        <v>819</v>
       </c>
       <c r="G81" s="27"/>
       <c r="H81" s="27"/>
@@ -12345,18 +12335,20 @@
     <row r="82" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A82" s="19"/>
       <c r="B82" s="30" t="s">
-        <v>891</v>
-      </c>
-      <c r="C82" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D82" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E82" s="27" t="s">
-        <v>892</v>
-      </c>
-      <c r="F82" s="27"/>
+        <v>820</v>
+      </c>
+      <c r="C82" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="E82" s="34" t="s">
+        <v>889</v>
+      </c>
+      <c r="F82" s="47" t="s">
+        <v>890</v>
+      </c>
       <c r="G82" s="27"/>
       <c r="H82" s="27"/>
       <c r="I82" s="27"/>
@@ -12370,7 +12362,7 @@
     <row r="83" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A83" s="19"/>
       <c r="B83" s="30" t="s">
-        <v>877</v>
+        <v>891</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>30</v>
@@ -12379,7 +12371,7 @@
         <v>363</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>878</v>
+        <v>892</v>
       </c>
       <c r="F83" s="27"/>
       <c r="G83" s="27"/>
@@ -12393,20 +12385,18 @@
       <c r="O83" s="22"/>
     </row>
     <row r="84" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A84" s="31" t="s">
-        <v>893</v>
-      </c>
+      <c r="A84" s="19"/>
       <c r="B84" s="30" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C84" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>253</v>
+        <v>363</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -12419,19 +12409,23 @@
       <c r="N84" s="23"/>
       <c r="O84" s="22"/>
     </row>
-    <row r="85" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A85" s="19"/>
-      <c r="B85" s="32" t="s">
-        <v>881</v>
-      </c>
-      <c r="C85" s="33" t="s">
+    <row r="85" s="1" customFormat="1" ht="68" customHeight="1" spans="1:15">
+      <c r="A85" s="31" t="s">
+        <v>893</v>
+      </c>
+      <c r="B85" s="30" t="s">
+        <v>879</v>
+      </c>
+      <c r="C85" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="34" t="s">
-        <v>620</v>
-      </c>
-      <c r="E85" s="34"/>
-      <c r="F85" s="47"/>
+      <c r="D85" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>880</v>
+      </c>
+      <c r="F85" s="27"/>
       <c r="G85" s="27"/>
       <c r="H85" s="27"/>
       <c r="I85" s="27"/>
@@ -12442,22 +12436,18 @@
       <c r="N85" s="23"/>
       <c r="O85" s="22"/>
     </row>
-    <row r="86" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
-      <c r="A86" s="19" t="s">
-        <v>894</v>
-      </c>
-      <c r="B86" s="30" t="s">
-        <v>793</v>
-      </c>
-      <c r="C86" s="26" t="s">
+    <row r="86" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A86" s="19"/>
+      <c r="B86" s="32" t="s">
+        <v>881</v>
+      </c>
+      <c r="C86" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D86" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E86" s="27" t="s">
-        <v>794</v>
-      </c>
+      <c r="D86" s="34" t="s">
+        <v>620</v>
+      </c>
+      <c r="E86" s="34"/>
       <c r="F86" s="47"/>
       <c r="G86" s="27"/>
       <c r="H86" s="27"/>
@@ -12469,23 +12459,23 @@
       <c r="N86" s="23"/>
       <c r="O86" s="22"/>
     </row>
-    <row r="87" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A87" s="19"/>
-      <c r="B87" s="32" t="s">
-        <v>800</v>
-      </c>
-      <c r="C87" s="33" t="s">
+    <row r="87" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
+      <c r="A87" s="19" t="s">
+        <v>894</v>
+      </c>
+      <c r="B87" s="30" t="s">
+        <v>793</v>
+      </c>
+      <c r="C87" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E87" s="34" t="s">
-        <v>801</v>
-      </c>
-      <c r="F87" s="47" t="s">
-        <v>802</v>
-      </c>
+      <c r="D87" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E87" s="27" t="s">
+        <v>794</v>
+      </c>
+      <c r="F87" s="47"/>
       <c r="G87" s="27"/>
       <c r="H87" s="27"/>
       <c r="I87" s="27"/>
@@ -12499,18 +12489,20 @@
     <row r="88" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A88" s="19"/>
       <c r="B88" s="32" t="s">
-        <v>835</v>
+        <v>800</v>
       </c>
       <c r="C88" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D88" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E88" s="27" t="s">
-        <v>836</v>
-      </c>
-      <c r="F88" s="47"/>
+        <v>707</v>
+      </c>
+      <c r="E88" s="34" t="s">
+        <v>801</v>
+      </c>
+      <c r="F88" s="47" t="s">
+        <v>802</v>
+      </c>
       <c r="G88" s="27"/>
       <c r="H88" s="27"/>
       <c r="I88" s="27"/>
@@ -12524,7 +12516,7 @@
     <row r="89" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A89" s="19"/>
       <c r="B89" s="32" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C89" s="33" t="s">
         <v>30</v>
@@ -12533,7 +12525,7 @@
         <v>363</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="F89" s="47"/>
       <c r="G89" s="27"/>
@@ -12548,21 +12540,19 @@
     </row>
     <row r="90" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A90" s="19"/>
-      <c r="B90" s="30" t="s">
-        <v>806</v>
+      <c r="B90" s="32" t="s">
+        <v>837</v>
       </c>
       <c r="C90" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D90" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E90" s="34" t="s">
-        <v>839</v>
-      </c>
-      <c r="F90" s="47" t="s">
-        <v>808</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="E90" s="27" t="s">
+        <v>838</v>
+      </c>
+      <c r="F90" s="47"/>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
       <c r="I90" s="27"/>
@@ -12576,19 +12566,19 @@
     <row r="91" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A91" s="19"/>
       <c r="B91" s="30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C91" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D91" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E91" s="34" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F91" s="47" t="s">
-        <v>841</v>
+        <v>808</v>
       </c>
       <c r="G91" s="27"/>
       <c r="H91" s="27"/>
@@ -12603,19 +12593,19 @@
     <row r="92" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A92" s="19"/>
       <c r="B92" s="30" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C92" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D92" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E92" s="28" t="s">
-        <v>842</v>
-      </c>
-      <c r="F92" s="27" t="s">
-        <v>813</v>
+        <v>471</v>
+      </c>
+      <c r="E92" s="34" t="s">
+        <v>840</v>
+      </c>
+      <c r="F92" s="47" t="s">
+        <v>841</v>
       </c>
       <c r="G92" s="27"/>
       <c r="H92" s="27"/>
@@ -12630,7 +12620,7 @@
     <row r="93" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A93" s="19"/>
       <c r="B93" s="30" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="C93" s="33" t="s">
         <v>30</v>
@@ -12639,10 +12629,10 @@
         <v>707</v>
       </c>
       <c r="E93" s="28" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F93" s="27" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="G93" s="27"/>
       <c r="H93" s="27"/>
@@ -12657,19 +12647,19 @@
     <row r="94" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A94" s="19"/>
       <c r="B94" s="30" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="C94" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D94" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E94" s="34" t="s">
-        <v>844</v>
-      </c>
-      <c r="F94" s="47" t="s">
-        <v>819</v>
+        <v>707</v>
+      </c>
+      <c r="E94" s="28" t="s">
+        <v>843</v>
+      </c>
+      <c r="F94" s="27" t="s">
+        <v>816</v>
       </c>
       <c r="G94" s="27"/>
       <c r="H94" s="27"/>
@@ -12684,19 +12674,19 @@
     <row r="95" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A95" s="19"/>
       <c r="B95" s="30" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C95" s="33" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D95" s="34" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="E95" s="34" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F95" s="47" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="G95" s="27"/>
       <c r="H95" s="27"/>
@@ -12711,19 +12701,19 @@
     <row r="96" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A96" s="19"/>
       <c r="B96" s="30" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D96" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E96" s="28" t="s">
-        <v>846</v>
-      </c>
-      <c r="F96" s="27" t="s">
-        <v>847</v>
+        <v>471</v>
+      </c>
+      <c r="E96" s="34" t="s">
+        <v>845</v>
+      </c>
+      <c r="F96" s="47" t="s">
+        <v>822</v>
       </c>
       <c r="G96" s="27"/>
       <c r="H96" s="27"/>
@@ -12737,18 +12727,20 @@
     </row>
     <row r="97" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A97" s="19"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="36" t="s">
-        <v>656</v>
-      </c>
-      <c r="E97" s="48" t="s">
-        <v>789</v>
-      </c>
-      <c r="F97" s="49" t="s">
-        <v>790</v>
+      <c r="B97" s="30" t="s">
+        <v>823</v>
+      </c>
+      <c r="C97" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>846</v>
+      </c>
+      <c r="F97" s="27" t="s">
+        <v>847</v>
       </c>
       <c r="G97" s="27"/>
       <c r="H97" s="27"/>
@@ -12762,20 +12754,18 @@
     </row>
     <row r="98" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A98" s="19"/>
-      <c r="B98" s="30" t="s">
-        <v>826</v>
-      </c>
-      <c r="C98" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D98" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E98" s="28" t="s">
-        <v>848</v>
-      </c>
-      <c r="F98" s="27" t="s">
-        <v>778</v>
+      <c r="B98" s="30"/>
+      <c r="C98" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="E98" s="48" t="s">
+        <v>789</v>
+      </c>
+      <c r="F98" s="49" t="s">
+        <v>790</v>
       </c>
       <c r="G98" s="27"/>
       <c r="H98" s="27"/>
@@ -12790,18 +12780,20 @@
     <row r="99" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A99" s="19"/>
       <c r="B99" s="30" t="s">
-        <v>828</v>
-      </c>
-      <c r="C99" s="26" t="s">
+        <v>826</v>
+      </c>
+      <c r="C99" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D99" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E99" s="27" t="s">
-        <v>829</v>
-      </c>
-      <c r="F99" s="27"/>
+      <c r="D99" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>848</v>
+      </c>
+      <c r="F99" s="27" t="s">
+        <v>778</v>
+      </c>
       <c r="G99" s="27"/>
       <c r="H99" s="27"/>
       <c r="I99" s="27"/>
@@ -12813,20 +12805,18 @@
       <c r="O99" s="22"/>
     </row>
     <row r="100" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A100" s="31" t="s">
-        <v>893</v>
-      </c>
-      <c r="B100" s="32" t="s">
-        <v>830</v>
-      </c>
-      <c r="C100" s="33" t="s">
+      <c r="A100" s="19"/>
+      <c r="B100" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="C100" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D100" s="34" t="s">
-        <v>253</v>
+      <c r="D100" s="27" t="s">
+        <v>363</v>
       </c>
       <c r="E100" s="27" t="s">
-        <v>895</v>
+        <v>829</v>
       </c>
       <c r="F100" s="27"/>
       <c r="G100" s="27"/>
@@ -12839,17 +12829,22 @@
       <c r="N100" s="23"/>
       <c r="O100" s="22"/>
     </row>
-    <row r="101" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B101" s="30" t="s">
-        <v>881</v>
-      </c>
-      <c r="C101" s="26" t="s">
+    <row r="101" s="1" customFormat="1" ht="86" customHeight="1" spans="1:15">
+      <c r="A101" s="31" t="s">
+        <v>893</v>
+      </c>
+      <c r="B101" s="32" t="s">
+        <v>830</v>
+      </c>
+      <c r="C101" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D101" s="27" t="s">
-        <v>620</v>
-      </c>
-      <c r="E101" s="27"/>
+      <c r="D101" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="E101" s="27" t="s">
+        <v>895</v>
+      </c>
       <c r="F101" s="27"/>
       <c r="G101" s="27"/>
       <c r="H101" s="27"/>
@@ -12861,25 +12856,18 @@
       <c r="N101" s="23"/>
       <c r="O101" s="22"/>
     </row>
-    <row r="102" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A102" s="19" t="s">
-        <v>896</v>
-      </c>
+    <row r="102" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B102" s="30" t="s">
-        <v>852</v>
-      </c>
-      <c r="C102" s="33" t="s">
+        <v>881</v>
+      </c>
+      <c r="C102" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D102" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E102" s="34" t="s">
-        <v>765</v>
-      </c>
-      <c r="F102" s="47" t="s">
-        <v>802</v>
-      </c>
+      <c r="D102" s="27" t="s">
+        <v>620</v>
+      </c>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
       <c r="G102" s="27"/>
       <c r="H102" s="27"/>
       <c r="I102" s="27"/>
@@ -12891,20 +12879,24 @@
       <c r="O102" s="22"/>
     </row>
     <row r="103" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A103" s="19"/>
+      <c r="A103" s="19" t="s">
+        <v>896</v>
+      </c>
       <c r="B103" s="30" t="s">
-        <v>897</v>
-      </c>
-      <c r="C103" s="26" t="s">
+        <v>852</v>
+      </c>
+      <c r="C103" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D103" s="27" t="s">
-        <v>600</v>
-      </c>
-      <c r="E103" s="27" t="s">
-        <v>898</v>
-      </c>
-      <c r="F103" s="27"/>
+      <c r="D103" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E103" s="34" t="s">
+        <v>765</v>
+      </c>
+      <c r="F103" s="47" t="s">
+        <v>802</v>
+      </c>
       <c r="G103" s="27"/>
       <c r="H103" s="27"/>
       <c r="I103" s="27"/>
@@ -12918,16 +12910,16 @@
     <row r="104" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A104" s="19"/>
       <c r="B104" s="30" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>253</v>
+        <v>600</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F104" s="27"/>
       <c r="G104" s="27"/>
@@ -12943,16 +12935,16 @@
     <row r="105" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A105" s="19"/>
       <c r="B105" s="30" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D105" s="27" t="s">
-        <v>363</v>
+        <v>253</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="F105" s="27"/>
       <c r="G105" s="27"/>
@@ -12968,7 +12960,7 @@
     <row r="106" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A106" s="19"/>
       <c r="B106" s="30" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C106" s="26" t="s">
         <v>30</v>
@@ -12977,7 +12969,7 @@
         <v>363</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="F106" s="27"/>
       <c r="G106" s="27"/>
@@ -12991,20 +12983,18 @@
       <c r="O106" s="22"/>
     </row>
     <row r="107" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A107" s="31" t="s">
-        <v>893</v>
-      </c>
+      <c r="A107" s="19"/>
       <c r="B107" s="30" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C107" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>253</v>
+        <v>363</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F107" s="27"/>
       <c r="G107" s="27"/>
@@ -13017,18 +13007,22 @@
       <c r="N107" s="23"/>
       <c r="O107" s="22"/>
     </row>
-    <row r="108" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A108" s="19"/>
+    <row r="108" s="1" customFormat="1" ht="71" customHeight="1" spans="1:15">
+      <c r="A108" s="31" t="s">
+        <v>893</v>
+      </c>
       <c r="B108" s="30" t="s">
-        <v>784</v>
+        <v>904</v>
       </c>
       <c r="C108" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D108" s="27" t="s">
-        <v>638</v>
-      </c>
-      <c r="E108" s="27"/>
+        <v>253</v>
+      </c>
+      <c r="E108" s="27" t="s">
+        <v>905</v>
+      </c>
       <c r="F108" s="27"/>
       <c r="G108" s="27"/>
       <c r="H108" s="27"/>
@@ -13042,9 +13036,15 @@
     </row>
     <row r="109" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A109" s="19"/>
-      <c r="B109" s="30"/>
-      <c r="C109" s="26"/>
-      <c r="D109" s="27"/>
+      <c r="B109" s="30" t="s">
+        <v>784</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D109" s="27" t="s">
+        <v>638</v>
+      </c>
       <c r="E109" s="27"/>
       <c r="F109" s="27"/>
       <c r="G109" s="27"/>
@@ -13110,7 +13110,7 @@
     </row>
     <row r="113" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A113" s="19"/>
-      <c r="B113" s="20"/>
+      <c r="B113" s="30"/>
       <c r="C113" s="26"/>
       <c r="D113" s="27"/>
       <c r="E113" s="27"/>
@@ -14604,6 +14604,23 @@
       <c r="N200" s="23"/>
       <c r="O200" s="22"/>
     </row>
+    <row r="201" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A201" s="19"/>
+      <c r="B201" s="20"/>
+      <c r="C201" s="26"/>
+      <c r="D201" s="27"/>
+      <c r="E201" s="27"/>
+      <c r="F201" s="27"/>
+      <c r="G201" s="27"/>
+      <c r="H201" s="27"/>
+      <c r="I201" s="27"/>
+      <c r="J201" s="61"/>
+      <c r="K201" s="22"/>
+      <c r="L201" s="23"/>
+      <c r="M201" s="21"/>
+      <c r="N201" s="23"/>
+      <c r="O201" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
@@ -14611,18 +14628,18 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N113:N200">
+  <conditionalFormatting sqref="N114:N201">
     <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N113,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N114,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N113,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N114,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N113,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N114,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N3:N112">
+  <conditionalFormatting sqref="N1 N3:N113">
     <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -14634,10 +14651,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C14 C15 C16 C17 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C74 C75 C76 C77 C78 C79 C80 C81 C82 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C105 C106 C12:C13 C18:C19 C72:C73 C83:C84 C103:C104 C107:C108 C109:C112 C113:C200">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C15 C16 C17 C18 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C75 C76 C77 C78 C79 C80 C81 C82 C83 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C106 C107 C13:C14 C19:C20 C73:C74 C84:C85 C104:C105 C108:C109 C110:C113 C114:C201">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D14 D15 D16 D17 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D74 D75 D76 D77 D78 D79 D80 D81 D82 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D105 D106 D12:D13 D18:D19 D72:D73 D83:D84 D103:D104 D107:D108 D109:D112 D113:D200">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D15 D16 D17 D18 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D75 D76 D77 D78 D79 D80 D81 D82 D83 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D106 D107 D13:D14 D19:D20 D73:D74 D84:D85 D104:D105 D108:D109 D110:D113 D114:D201">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Invoice and Add Category script
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-AddCategory.xlsx
+++ b/tests/artifact/script/UI-AddCategory.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1957" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="967">
   <si>
     <t>target</t>
   </si>
@@ -2784,15 +2784,15 @@
     <t>${specification.title.values.xpath}</t>
   </si>
   <si>
+    <t>${rowcountvalue}</t>
+  </si>
+  <si>
     <t>Store the counter value as 0</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>${rowcountvalue}</t>
-  </si>
-  <si>
     <t>Increase the Counter value as 1</t>
   </si>
   <si>
@@ -2811,7 +2811,7 @@
     <t>spectitlevalue</t>
   </si>
   <si>
-    <t>(${specification.title.values.xpath})[${counter}]</t>
+    <t>(${specification.title.values.xpath})[1]</t>
   </si>
   <si>
     <t>Compare Expected and Actual values</t>
@@ -3757,7 +3757,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4002,6 +4002,10 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7240,7 +7244,7 @@
       </c>
     </row>
     <row r="5" s="3" customFormat="1" ht="40" customHeight="1" spans="1:15">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="76" t="s">
         <v>747</v>
       </c>
       <c r="B5" s="30" t="s">
@@ -7255,7 +7259,7 @@
       <c r="E5" s="36" t="s">
         <v>749</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="77" t="s">
         <v>750</v>
       </c>
       <c r="G5" s="27"/>
@@ -7269,13 +7273,13 @@
       <c r="O5" s="58"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A6" s="77"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="80"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="81"/>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
       <c r="J6" s="57"/>
@@ -7286,9 +7290,9 @@
       <c r="O6" s="58"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A7" s="77"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="71"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
@@ -7303,12 +7307,12 @@
       <c r="O7" s="58"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A8" s="77"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="84"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="85"/>
       <c r="G8" s="29"/>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
@@ -7440,7 +7444,7 @@
     </row>
     <row r="16" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="19"/>
-      <c r="B16" s="85"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="26"/>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
@@ -10435,10 +10439,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O241"/>
+  <dimension ref="A1:O237"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -12779,21 +12783,17 @@
       <c r="O88" s="22"/>
     </row>
     <row r="89" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B89" s="62" t="s">
-        <v>906</v>
-      </c>
+      <c r="B89" s="62"/>
       <c r="C89" s="66" t="s">
         <v>5</v>
       </c>
       <c r="D89" s="67" t="s">
-        <v>471</v>
+        <v>536</v>
       </c>
       <c r="E89" s="67" t="s">
-        <v>773</v>
-      </c>
-      <c r="F89" s="68" t="s">
-        <v>774</v>
-      </c>
+        <v>906</v>
+      </c>
+      <c r="F89" s="68"/>
       <c r="G89" s="27"/>
       <c r="H89" s="27"/>
       <c r="I89" s="27"/>
@@ -12805,18 +12805,20 @@
       <c r="O89" s="22"/>
     </row>
     <row r="90" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B90" s="62"/>
+      <c r="B90" s="62" t="s">
+        <v>907</v>
+      </c>
       <c r="C90" s="66" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="67" t="s">
-        <v>465</v>
-      </c>
-      <c r="E90" s="64" t="s">
-        <v>907</v>
-      </c>
-      <c r="F90" s="64" t="s">
-        <v>776</v>
+        <v>471</v>
+      </c>
+      <c r="E90" s="67" t="s">
+        <v>773</v>
+      </c>
+      <c r="F90" s="68" t="s">
+        <v>774</v>
       </c>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
@@ -12833,14 +12835,14 @@
       <c r="C91" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="E91" s="67" t="s">
-        <v>777</v>
+      <c r="D91" s="67" t="s">
+        <v>465</v>
+      </c>
+      <c r="E91" s="64" t="s">
+        <v>908</v>
       </c>
       <c r="F91" s="64" t="s">
-        <v>908</v>
+        <v>776</v>
       </c>
       <c r="G91" s="27"/>
       <c r="H91" s="27"/>
@@ -12853,20 +12855,18 @@
       <c r="O91" s="22"/>
     </row>
     <row r="92" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B92" s="62" t="s">
-        <v>909</v>
-      </c>
+      <c r="B92" s="62"/>
       <c r="C92" s="66" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D92" s="69" t="s">
-        <v>302</v>
+        <v>49</v>
       </c>
       <c r="E92" s="67" t="s">
-        <v>773</v>
-      </c>
-      <c r="F92" s="68" t="s">
-        <v>780</v>
+        <v>777</v>
+      </c>
+      <c r="F92" s="64" t="s">
+        <v>775</v>
       </c>
       <c r="G92" s="27"/>
       <c r="H92" s="27"/>
@@ -12879,18 +12879,20 @@
       <c r="O92" s="22"/>
     </row>
     <row r="93" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B93" s="62"/>
-      <c r="C93" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="D93" s="64" t="s">
-        <v>614</v>
-      </c>
-      <c r="E93" s="64" t="s">
-        <v>910</v>
-      </c>
-      <c r="F93" s="64" t="s">
-        <v>911</v>
+      <c r="B93" s="62" t="s">
+        <v>909</v>
+      </c>
+      <c r="C93" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="69" t="s">
+        <v>302</v>
+      </c>
+      <c r="E93" s="67" t="s">
+        <v>773</v>
+      </c>
+      <c r="F93" s="68" t="s">
+        <v>780</v>
       </c>
       <c r="G93" s="27"/>
       <c r="H93" s="27"/>
@@ -12904,16 +12906,18 @@
     </row>
     <row r="94" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B94" s="62"/>
-      <c r="C94" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="64" t="s">
-        <v>536</v>
-      </c>
-      <c r="E94" s="64" t="s">
-        <v>912</v>
-      </c>
-      <c r="F94" s="64"/>
+      <c r="C94" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D94" s="41" t="s">
+        <v>614</v>
+      </c>
+      <c r="E94" s="41" t="s">
+        <v>910</v>
+      </c>
+      <c r="F94" s="41" t="s">
+        <v>911</v>
+      </c>
       <c r="G94" s="27"/>
       <c r="H94" s="27"/>
       <c r="I94" s="27"/>
@@ -12925,21 +12929,17 @@
       <c r="O94" s="22"/>
     </row>
     <row r="95" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B95" s="62" t="s">
-        <v>913</v>
-      </c>
-      <c r="C95" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="D95" s="64" t="s">
-        <v>493</v>
-      </c>
-      <c r="E95" s="64" t="s">
-        <v>914</v>
-      </c>
-      <c r="F95" s="64" t="s">
-        <v>915</v>
-      </c>
+      <c r="B95" s="62"/>
+      <c r="C95" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" s="41" t="s">
+        <v>536</v>
+      </c>
+      <c r="E95" s="41" t="s">
+        <v>912</v>
+      </c>
+      <c r="F95" s="41"/>
       <c r="G95" s="27"/>
       <c r="H95" s="27"/>
       <c r="I95" s="27"/>
@@ -12952,19 +12952,19 @@
     </row>
     <row r="96" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B96" s="62" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="C96" s="63" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D96" s="64" t="s">
-        <v>49</v>
+        <v>493</v>
       </c>
       <c r="E96" s="64" t="s">
-        <v>882</v>
+        <v>914</v>
       </c>
       <c r="F96" s="64" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="G96" s="27"/>
       <c r="H96" s="27"/>
@@ -12978,18 +12978,20 @@
     </row>
     <row r="97" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B97" s="62" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C97" s="63" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D97" s="64" t="s">
-        <v>363</v>
+        <v>49</v>
       </c>
       <c r="E97" s="64" t="s">
-        <v>919</v>
-      </c>
-      <c r="F97" s="64"/>
+        <v>882</v>
+      </c>
+      <c r="F97" s="64" t="s">
+        <v>917</v>
+      </c>
       <c r="G97" s="27"/>
       <c r="H97" s="27"/>
       <c r="I97" s="27"/>
@@ -13000,43 +13002,50 @@
       <c r="N97" s="23"/>
       <c r="O97" s="22"/>
     </row>
-    <row r="98" s="1" customFormat="1" ht="37" customHeight="1" spans="2:15">
-      <c r="B98" s="62" t="s">
-        <v>920</v>
-      </c>
-      <c r="C98" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="64" t="s">
-        <v>536</v>
-      </c>
-      <c r="E98" s="64" t="s">
-        <v>921</v>
+    <row r="98" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
+      <c r="B98" s="70" t="s">
+        <v>918</v>
+      </c>
+      <c r="C98" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="E98" s="41" t="s">
+        <v>919</v>
       </c>
       <c r="F98" s="64"/>
       <c r="G98" s="27"/>
       <c r="H98" s="27"/>
       <c r="I98" s="27"/>
-      <c r="J98" s="1" t="s">
-        <v>922</v>
-      </c>
+      <c r="J98" s="61"/>
       <c r="K98" s="22"/>
       <c r="L98" s="23"/>
       <c r="M98" s="21"/>
       <c r="N98" s="23"/>
       <c r="O98" s="22"/>
     </row>
-    <row r="99" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A99" s="19"/>
-      <c r="B99" s="30"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="34"/>
-      <c r="E99" s="34"/>
-      <c r="F99" s="47"/>
+    <row r="99" s="1" customFormat="1" ht="37" customHeight="1" spans="2:15">
+      <c r="B99" s="62" t="s">
+        <v>920</v>
+      </c>
+      <c r="C99" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="64" t="s">
+        <v>536</v>
+      </c>
+      <c r="E99" s="64" t="s">
+        <v>921</v>
+      </c>
+      <c r="F99" s="64"/>
       <c r="G99" s="27"/>
       <c r="H99" s="27"/>
       <c r="I99" s="27"/>
-      <c r="J99" s="61"/>
+      <c r="J99" s="1" t="s">
+        <v>922</v>
+      </c>
       <c r="K99" s="22"/>
       <c r="L99" s="23"/>
       <c r="M99" s="21"/>
@@ -13130,11 +13139,21 @@
     </row>
     <row r="105" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A105" s="19"/>
-      <c r="B105" s="30"/>
-      <c r="C105" s="33"/>
-      <c r="D105" s="34"/>
-      <c r="E105" s="34"/>
-      <c r="F105" s="47"/>
+      <c r="B105" s="30" t="s">
+        <v>809</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D105" s="34" t="s">
+        <v>483</v>
+      </c>
+      <c r="E105" s="34" t="s">
+        <v>923</v>
+      </c>
+      <c r="F105" s="47" t="s">
+        <v>811</v>
+      </c>
       <c r="G105" s="27"/>
       <c r="H105" s="27"/>
       <c r="I105" s="27"/>
@@ -13147,11 +13166,21 @@
     </row>
     <row r="106" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A106" s="19"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="33"/>
-      <c r="D106" s="34"/>
-      <c r="E106" s="34"/>
-      <c r="F106" s="47"/>
+      <c r="B106" s="30" t="s">
+        <v>812</v>
+      </c>
+      <c r="C106" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="E106" s="34" t="s">
+        <v>924</v>
+      </c>
+      <c r="F106" s="47" t="s">
+        <v>925</v>
+      </c>
       <c r="G106" s="27"/>
       <c r="H106" s="27"/>
       <c r="I106" s="27"/>
@@ -13164,11 +13193,19 @@
     </row>
     <row r="107" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A107" s="19"/>
-      <c r="B107" s="30"/>
-      <c r="C107" s="33"/>
-      <c r="D107" s="34"/>
-      <c r="E107" s="34"/>
-      <c r="F107" s="47"/>
+      <c r="B107" s="30" t="s">
+        <v>926</v>
+      </c>
+      <c r="C107" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E107" s="27" t="s">
+        <v>927</v>
+      </c>
+      <c r="F107" s="27"/>
       <c r="G107" s="27"/>
       <c r="H107" s="27"/>
       <c r="I107" s="27"/>
@@ -13181,11 +13218,21 @@
     </row>
     <row r="108" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A108" s="19"/>
-      <c r="B108" s="30"/>
-      <c r="C108" s="33"/>
-      <c r="D108" s="34"/>
-      <c r="E108" s="34"/>
-      <c r="F108" s="47"/>
+      <c r="B108" s="30" t="s">
+        <v>820</v>
+      </c>
+      <c r="C108" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D108" s="34" t="s">
+        <v>483</v>
+      </c>
+      <c r="E108" s="34" t="s">
+        <v>928</v>
+      </c>
+      <c r="F108" s="47" t="s">
+        <v>822</v>
+      </c>
       <c r="G108" s="27"/>
       <c r="H108" s="27"/>
       <c r="I108" s="27"/>
@@ -13199,19 +13246,19 @@
     <row r="109" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A109" s="19"/>
       <c r="B109" s="30" t="s">
-        <v>809</v>
+        <v>823</v>
       </c>
       <c r="C109" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D109" s="34" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="E109" s="34" t="s">
-        <v>923</v>
+        <v>929</v>
       </c>
       <c r="F109" s="47" t="s">
-        <v>811</v>
+        <v>930</v>
       </c>
       <c r="G109" s="27"/>
       <c r="H109" s="27"/>
@@ -13226,20 +13273,18 @@
     <row r="110" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A110" s="19"/>
       <c r="B110" s="30" t="s">
-        <v>812</v>
-      </c>
-      <c r="C110" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D110" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="E110" s="34" t="s">
-        <v>924</v>
-      </c>
-      <c r="F110" s="47" t="s">
-        <v>925</v>
-      </c>
+        <v>931</v>
+      </c>
+      <c r="C110" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D110" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E110" s="27" t="s">
+        <v>932</v>
+      </c>
+      <c r="F110" s="27"/>
       <c r="G110" s="27"/>
       <c r="H110" s="27"/>
       <c r="I110" s="27"/>
@@ -13253,7 +13298,7 @@
     <row r="111" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A111" s="19"/>
       <c r="B111" s="30" t="s">
-        <v>926</v>
+        <v>894</v>
       </c>
       <c r="C111" s="26" t="s">
         <v>30</v>
@@ -13262,7 +13307,7 @@
         <v>363</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>927</v>
+        <v>895</v>
       </c>
       <c r="F111" s="27"/>
       <c r="G111" s="27"/>
@@ -13275,23 +13320,21 @@
       <c r="N111" s="23"/>
       <c r="O111" s="22"/>
     </row>
-    <row r="112" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A112" s="19"/>
-      <c r="B112" s="30" t="s">
-        <v>820</v>
-      </c>
-      <c r="C112" s="33" t="s">
+    <row r="112" s="1" customFormat="1" ht="68" customHeight="1" spans="1:15">
+      <c r="A112" s="31"/>
+      <c r="B112" s="71" t="s">
+        <v>933</v>
+      </c>
+      <c r="C112" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="D112" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E112" s="34" t="s">
-        <v>928</v>
-      </c>
-      <c r="F112" s="47" t="s">
-        <v>822</v>
-      </c>
+      <c r="D112" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E112" s="29" t="s">
+        <v>934</v>
+      </c>
+      <c r="F112" s="27"/>
       <c r="G112" s="27"/>
       <c r="H112" s="27"/>
       <c r="I112" s="27"/>
@@ -13302,22 +13345,22 @@
       <c r="N112" s="23"/>
       <c r="O112" s="22"/>
     </row>
-    <row r="113" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="113" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
       <c r="A113" s="19"/>
-      <c r="B113" s="30" t="s">
-        <v>823</v>
-      </c>
-      <c r="C113" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D113" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="E113" s="34" t="s">
-        <v>929</v>
-      </c>
-      <c r="F113" s="47" t="s">
-        <v>930</v>
+      <c r="B113" s="62" t="s">
+        <v>833</v>
+      </c>
+      <c r="C113" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D113" s="64" t="s">
+        <v>493</v>
+      </c>
+      <c r="E113" s="64" t="s">
+        <v>935</v>
+      </c>
+      <c r="F113" s="65" t="s">
+        <v>835</v>
       </c>
       <c r="G113" s="27"/>
       <c r="H113" s="27"/>
@@ -13329,21 +13372,23 @@
       <c r="N113" s="23"/>
       <c r="O113" s="22"/>
     </row>
-    <row r="114" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="114" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
       <c r="A114" s="19"/>
-      <c r="B114" s="30" t="s">
-        <v>931</v>
-      </c>
-      <c r="C114" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D114" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E114" s="27" t="s">
-        <v>932</v>
-      </c>
-      <c r="F114" s="27"/>
+      <c r="B114" s="62" t="s">
+        <v>836</v>
+      </c>
+      <c r="C114" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="64" t="s">
+        <v>471</v>
+      </c>
+      <c r="E114" s="64" t="s">
+        <v>936</v>
+      </c>
+      <c r="F114" s="64" t="s">
+        <v>898</v>
+      </c>
       <c r="G114" s="27"/>
       <c r="H114" s="27"/>
       <c r="I114" s="27"/>
@@ -13354,21 +13399,23 @@
       <c r="N114" s="23"/>
       <c r="O114" s="22"/>
     </row>
-    <row r="115" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="115" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
       <c r="A115" s="19"/>
-      <c r="B115" s="30" t="s">
-        <v>894</v>
-      </c>
-      <c r="C115" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D115" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E115" s="27" t="s">
-        <v>895</v>
-      </c>
-      <c r="F115" s="27"/>
+      <c r="B115" s="62" t="s">
+        <v>839</v>
+      </c>
+      <c r="C115" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E115" s="64" t="s">
+        <v>937</v>
+      </c>
+      <c r="F115" s="64" t="s">
+        <v>938</v>
+      </c>
       <c r="G115" s="27"/>
       <c r="H115" s="27"/>
       <c r="I115" s="27"/>
@@ -13379,21 +13426,19 @@
       <c r="N115" s="23"/>
       <c r="O115" s="22"/>
     </row>
-    <row r="116" s="1" customFormat="1" ht="68" customHeight="1" spans="1:15">
-      <c r="A116" s="31"/>
-      <c r="B116" s="70" t="s">
-        <v>933</v>
-      </c>
-      <c r="C116" s="71" t="s">
+    <row r="116" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
+      <c r="A116" s="19"/>
+      <c r="B116" s="32" t="s">
+        <v>901</v>
+      </c>
+      <c r="C116" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D116" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="E116" s="29" t="s">
-        <v>934</v>
-      </c>
-      <c r="F116" s="27"/>
+      <c r="D116" s="34" t="s">
+        <v>620</v>
+      </c>
+      <c r="E116" s="27"/>
+      <c r="F116" s="47"/>
       <c r="G116" s="27"/>
       <c r="H116" s="27"/>
       <c r="I116" s="27"/>
@@ -13405,22 +13450,22 @@
       <c r="O116" s="22"/>
     </row>
     <row r="117" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
-      <c r="A117" s="19"/>
-      <c r="B117" s="62" t="s">
-        <v>833</v>
-      </c>
-      <c r="C117" s="63" t="s">
+      <c r="A117" s="19" t="s">
+        <v>939</v>
+      </c>
+      <c r="B117" s="30" t="s">
+        <v>795</v>
+      </c>
+      <c r="C117" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D117" s="64" t="s">
-        <v>493</v>
-      </c>
-      <c r="E117" s="64" t="s">
-        <v>935</v>
-      </c>
-      <c r="F117" s="65" t="s">
-        <v>835</v>
-      </c>
+      <c r="D117" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E117" s="27" t="s">
+        <v>764</v>
+      </c>
+      <c r="F117" s="47"/>
       <c r="G117" s="27"/>
       <c r="H117" s="27"/>
       <c r="I117" s="27"/>
@@ -13431,22 +13476,22 @@
       <c r="N117" s="23"/>
       <c r="O117" s="22"/>
     </row>
-    <row r="118" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
+    <row r="118" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A118" s="19"/>
-      <c r="B118" s="62" t="s">
-        <v>836</v>
-      </c>
-      <c r="C118" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D118" s="64" t="s">
-        <v>471</v>
-      </c>
-      <c r="E118" s="64" t="s">
-        <v>936</v>
-      </c>
-      <c r="F118" s="64" t="s">
-        <v>898</v>
+      <c r="B118" s="32" t="s">
+        <v>801</v>
+      </c>
+      <c r="C118" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D118" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E118" s="34" t="s">
+        <v>802</v>
+      </c>
+      <c r="F118" s="47" t="s">
+        <v>803</v>
       </c>
       <c r="G118" s="27"/>
       <c r="H118" s="27"/>
@@ -13458,23 +13503,21 @@
       <c r="N118" s="23"/>
       <c r="O118" s="22"/>
     </row>
-    <row r="119" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
+    <row r="119" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A119" s="19"/>
-      <c r="B119" s="62" t="s">
-        <v>839</v>
-      </c>
-      <c r="C119" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D119" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="E119" s="64" t="s">
-        <v>937</v>
-      </c>
-      <c r="F119" s="64" t="s">
-        <v>938</v>
-      </c>
+      <c r="B119" s="32" t="s">
+        <v>845</v>
+      </c>
+      <c r="C119" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D119" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="E119" s="27" t="s">
+        <v>846</v>
+      </c>
+      <c r="F119" s="47"/>
       <c r="G119" s="27"/>
       <c r="H119" s="27"/>
       <c r="I119" s="27"/>
@@ -13485,18 +13528,20 @@
       <c r="N119" s="23"/>
       <c r="O119" s="22"/>
     </row>
-    <row r="120" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
+    <row r="120" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A120" s="19"/>
       <c r="B120" s="32" t="s">
-        <v>901</v>
+        <v>847</v>
       </c>
       <c r="C120" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D120" s="34" t="s">
-        <v>620</v>
-      </c>
-      <c r="E120" s="27"/>
+        <v>363</v>
+      </c>
+      <c r="E120" s="27" t="s">
+        <v>848</v>
+      </c>
       <c r="F120" s="47"/>
       <c r="G120" s="27"/>
       <c r="H120" s="27"/>
@@ -13508,23 +13553,23 @@
       <c r="N120" s="23"/>
       <c r="O120" s="22"/>
     </row>
-    <row r="121" s="1" customFormat="1" ht="33" customHeight="1" spans="1:15">
-      <c r="A121" s="19" t="s">
-        <v>939</v>
-      </c>
+    <row r="121" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A121" s="19"/>
       <c r="B121" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="C121" s="26" t="s">
+        <v>809</v>
+      </c>
+      <c r="C121" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D121" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E121" s="27" t="s">
-        <v>764</v>
-      </c>
-      <c r="F121" s="47"/>
+      <c r="D121" s="34" t="s">
+        <v>483</v>
+      </c>
+      <c r="E121" s="34" t="s">
+        <v>849</v>
+      </c>
+      <c r="F121" s="47" t="s">
+        <v>811</v>
+      </c>
       <c r="G121" s="27"/>
       <c r="H121" s="27"/>
       <c r="I121" s="27"/>
@@ -13537,20 +13582,20 @@
     </row>
     <row r="122" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A122" s="19"/>
-      <c r="B122" s="32" t="s">
-        <v>801</v>
+      <c r="B122" s="30" t="s">
+        <v>812</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D122" s="34" t="s">
-        <v>707</v>
+        <v>471</v>
       </c>
       <c r="E122" s="34" t="s">
-        <v>802</v>
+        <v>850</v>
       </c>
       <c r="F122" s="47" t="s">
-        <v>803</v>
+        <v>851</v>
       </c>
       <c r="G122" s="27"/>
       <c r="H122" s="27"/>
@@ -13564,19 +13609,21 @@
     </row>
     <row r="123" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A123" s="19"/>
-      <c r="B123" s="32" t="s">
-        <v>845</v>
+      <c r="B123" s="30" t="s">
+        <v>814</v>
       </c>
       <c r="C123" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D123" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E123" s="27" t="s">
-        <v>846</v>
-      </c>
-      <c r="F123" s="47"/>
+        <v>707</v>
+      </c>
+      <c r="E123" s="28" t="s">
+        <v>852</v>
+      </c>
+      <c r="F123" s="27" t="s">
+        <v>816</v>
+      </c>
       <c r="G123" s="27"/>
       <c r="H123" s="27"/>
       <c r="I123" s="27"/>
@@ -13589,19 +13636,21 @@
     </row>
     <row r="124" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A124" s="19"/>
-      <c r="B124" s="32" t="s">
-        <v>847</v>
+      <c r="B124" s="30" t="s">
+        <v>817</v>
       </c>
       <c r="C124" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D124" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E124" s="27" t="s">
-        <v>848</v>
-      </c>
-      <c r="F124" s="47"/>
+        <v>707</v>
+      </c>
+      <c r="E124" s="28" t="s">
+        <v>853</v>
+      </c>
+      <c r="F124" s="27" t="s">
+        <v>819</v>
+      </c>
       <c r="G124" s="27"/>
       <c r="H124" s="27"/>
       <c r="I124" s="27"/>
@@ -13615,7 +13664,7 @@
     <row r="125" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A125" s="19"/>
       <c r="B125" s="30" t="s">
-        <v>809</v>
+        <v>820</v>
       </c>
       <c r="C125" s="33" t="s">
         <v>30</v>
@@ -13624,10 +13673,10 @@
         <v>483</v>
       </c>
       <c r="E125" s="34" t="s">
-        <v>849</v>
+        <v>854</v>
       </c>
       <c r="F125" s="47" t="s">
-        <v>811</v>
+        <v>822</v>
       </c>
       <c r="G125" s="27"/>
       <c r="H125" s="27"/>
@@ -13642,7 +13691,7 @@
     <row r="126" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A126" s="19"/>
       <c r="B126" s="30" t="s">
-        <v>812</v>
+        <v>823</v>
       </c>
       <c r="C126" s="33" t="s">
         <v>5</v>
@@ -13651,10 +13700,10 @@
         <v>471</v>
       </c>
       <c r="E126" s="34" t="s">
-        <v>850</v>
+        <v>855</v>
       </c>
       <c r="F126" s="47" t="s">
-        <v>851</v>
+        <v>825</v>
       </c>
       <c r="G126" s="27"/>
       <c r="H126" s="27"/>
@@ -13669,7 +13718,7 @@
     <row r="127" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A127" s="19"/>
       <c r="B127" s="30" t="s">
-        <v>814</v>
+        <v>826</v>
       </c>
       <c r="C127" s="33" t="s">
         <v>30</v>
@@ -13678,10 +13727,10 @@
         <v>707</v>
       </c>
       <c r="E127" s="28" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="F127" s="27" t="s">
-        <v>816</v>
+        <v>858</v>
       </c>
       <c r="G127" s="27"/>
       <c r="H127" s="27"/>
@@ -13695,20 +13744,18 @@
     </row>
     <row r="128" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A128" s="19"/>
-      <c r="B128" s="30" t="s">
-        <v>817</v>
-      </c>
-      <c r="C128" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D128" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E128" s="28" t="s">
-        <v>853</v>
-      </c>
-      <c r="F128" s="27" t="s">
-        <v>819</v>
+      <c r="B128" s="30"/>
+      <c r="C128" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="E128" s="48" t="s">
+        <v>791</v>
+      </c>
+      <c r="F128" s="49" t="s">
+        <v>792</v>
       </c>
       <c r="G128" s="27"/>
       <c r="H128" s="27"/>
@@ -13723,19 +13770,19 @@
     <row r="129" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A129" s="19"/>
       <c r="B129" s="30" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="C129" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D129" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="E129" s="34" t="s">
-        <v>854</v>
-      </c>
-      <c r="F129" s="47" t="s">
-        <v>822</v>
+        <v>707</v>
+      </c>
+      <c r="E129" s="28" t="s">
+        <v>859</v>
+      </c>
+      <c r="F129" s="27" t="s">
+        <v>780</v>
       </c>
       <c r="G129" s="27"/>
       <c r="H129" s="27"/>
@@ -13750,20 +13797,18 @@
     <row r="130" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A130" s="19"/>
       <c r="B130" s="30" t="s">
-        <v>823</v>
-      </c>
-      <c r="C130" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D130" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="E130" s="34" t="s">
-        <v>855</v>
-      </c>
-      <c r="F130" s="47" t="s">
-        <v>825</v>
-      </c>
+        <v>831</v>
+      </c>
+      <c r="C130" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D130" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E130" s="27" t="s">
+        <v>832</v>
+      </c>
+      <c r="F130" s="27"/>
       <c r="G130" s="27"/>
       <c r="H130" s="27"/>
       <c r="I130" s="27"/>
@@ -13774,23 +13819,21 @@
       <c r="N130" s="23"/>
       <c r="O130" s="22"/>
     </row>
-    <row r="131" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A131" s="19"/>
-      <c r="B131" s="30" t="s">
-        <v>826</v>
-      </c>
-      <c r="C131" s="33" t="s">
+    <row r="131" s="1" customFormat="1" ht="86" customHeight="1" spans="1:15">
+      <c r="A131" s="31"/>
+      <c r="B131" s="73" t="s">
+        <v>940</v>
+      </c>
+      <c r="C131" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="D131" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E131" s="28" t="s">
-        <v>857</v>
-      </c>
-      <c r="F131" s="27" t="s">
-        <v>858</v>
-      </c>
+      <c r="D131" s="75" t="s">
+        <v>253</v>
+      </c>
+      <c r="E131" s="29" t="s">
+        <v>941</v>
+      </c>
+      <c r="F131" s="27"/>
       <c r="G131" s="27"/>
       <c r="H131" s="27"/>
       <c r="I131" s="27"/>
@@ -13801,20 +13844,21 @@
       <c r="N131" s="23"/>
       <c r="O131" s="22"/>
     </row>
-    <row r="132" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A132" s="19"/>
-      <c r="B132" s="30"/>
-      <c r="C132" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D132" s="36" t="s">
-        <v>656</v>
-      </c>
-      <c r="E132" s="48" t="s">
-        <v>791</v>
-      </c>
-      <c r="F132" s="49" t="s">
-        <v>792</v>
+    <row r="132" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
+      <c r="B132" s="62" t="s">
+        <v>833</v>
+      </c>
+      <c r="C132" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D132" s="64" t="s">
+        <v>493</v>
+      </c>
+      <c r="E132" s="64" t="s">
+        <v>942</v>
+      </c>
+      <c r="F132" s="65" t="s">
+        <v>835</v>
       </c>
       <c r="G132" s="27"/>
       <c r="H132" s="27"/>
@@ -13826,22 +13870,21 @@
       <c r="N132" s="23"/>
       <c r="O132" s="22"/>
     </row>
-    <row r="133" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A133" s="19"/>
-      <c r="B133" s="30" t="s">
-        <v>829</v>
-      </c>
-      <c r="C133" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D133" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E133" s="28" t="s">
-        <v>859</v>
-      </c>
-      <c r="F133" s="27" t="s">
-        <v>780</v>
+    <row r="133" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
+      <c r="B133" s="62" t="s">
+        <v>836</v>
+      </c>
+      <c r="C133" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133" s="64" t="s">
+        <v>471</v>
+      </c>
+      <c r="E133" s="64" t="s">
+        <v>943</v>
+      </c>
+      <c r="F133" s="64" t="s">
+        <v>944</v>
       </c>
       <c r="G133" s="27"/>
       <c r="H133" s="27"/>
@@ -13853,21 +13896,22 @@
       <c r="N133" s="23"/>
       <c r="O133" s="22"/>
     </row>
-    <row r="134" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A134" s="19"/>
-      <c r="B134" s="30" t="s">
-        <v>831</v>
-      </c>
-      <c r="C134" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D134" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E134" s="27" t="s">
-        <v>832</v>
-      </c>
-      <c r="F134" s="27"/>
+    <row r="134" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
+      <c r="B134" s="62" t="s">
+        <v>839</v>
+      </c>
+      <c r="C134" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E134" s="64" t="s">
+        <v>945</v>
+      </c>
+      <c r="F134" s="64" t="s">
+        <v>946</v>
+      </c>
       <c r="G134" s="27"/>
       <c r="H134" s="27"/>
       <c r="I134" s="27"/>
@@ -13878,20 +13922,17 @@
       <c r="N134" s="23"/>
       <c r="O134" s="22"/>
     </row>
-    <row r="135" s="1" customFormat="1" ht="86" customHeight="1" spans="1:15">
-      <c r="A135" s="31"/>
-      <c r="B135" s="72" t="s">
-        <v>940</v>
-      </c>
-      <c r="C135" s="73" t="s">
+    <row r="135" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
+      <c r="B135" s="30" t="s">
+        <v>901</v>
+      </c>
+      <c r="C135" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D135" s="74" t="s">
-        <v>253</v>
-      </c>
-      <c r="E135" s="29" t="s">
-        <v>941</v>
-      </c>
+      <c r="D135" s="27" t="s">
+        <v>620</v>
+      </c>
+      <c r="E135" s="27"/>
       <c r="F135" s="27"/>
       <c r="G135" s="27"/>
       <c r="H135" s="27"/>
@@ -13903,21 +13944,24 @@
       <c r="N135" s="23"/>
       <c r="O135" s="22"/>
     </row>
-    <row r="136" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B136" s="62" t="s">
-        <v>833</v>
-      </c>
-      <c r="C136" s="63" t="s">
+    <row r="136" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A136" s="19" t="s">
+        <v>947</v>
+      </c>
+      <c r="B136" s="30" t="s">
+        <v>867</v>
+      </c>
+      <c r="C136" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D136" s="64" t="s">
-        <v>493</v>
-      </c>
-      <c r="E136" s="64" t="s">
-        <v>942</v>
-      </c>
-      <c r="F136" s="65" t="s">
-        <v>835</v>
+      <c r="D136" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="E136" s="34" t="s">
+        <v>767</v>
+      </c>
+      <c r="F136" s="47" t="s">
+        <v>803</v>
       </c>
       <c r="G136" s="27"/>
       <c r="H136" s="27"/>
@@ -13929,22 +13973,21 @@
       <c r="N136" s="23"/>
       <c r="O136" s="22"/>
     </row>
-    <row r="137" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B137" s="62" t="s">
-        <v>836</v>
-      </c>
-      <c r="C137" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D137" s="64" t="s">
-        <v>471</v>
-      </c>
-      <c r="E137" s="64" t="s">
-        <v>943</v>
-      </c>
-      <c r="F137" s="64" t="s">
-        <v>944</v>
-      </c>
+    <row r="137" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A137" s="19"/>
+      <c r="B137" s="30" t="s">
+        <v>948</v>
+      </c>
+      <c r="C137" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D137" s="27" t="s">
+        <v>600</v>
+      </c>
+      <c r="E137" s="27" t="s">
+        <v>949</v>
+      </c>
+      <c r="F137" s="27"/>
       <c r="G137" s="27"/>
       <c r="H137" s="27"/>
       <c r="I137" s="27"/>
@@ -13955,22 +13998,21 @@
       <c r="N137" s="23"/>
       <c r="O137" s="22"/>
     </row>
-    <row r="138" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B138" s="62" t="s">
-        <v>839</v>
-      </c>
-      <c r="C138" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D138" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="E138" s="64" t="s">
-        <v>945</v>
-      </c>
-      <c r="F138" s="64" t="s">
-        <v>946</v>
-      </c>
+    <row r="138" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A138" s="19"/>
+      <c r="B138" s="30" t="s">
+        <v>950</v>
+      </c>
+      <c r="C138" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D138" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E138" s="27" t="s">
+        <v>951</v>
+      </c>
+      <c r="F138" s="27"/>
       <c r="G138" s="27"/>
       <c r="H138" s="27"/>
       <c r="I138" s="27"/>
@@ -13981,17 +14023,20 @@
       <c r="N138" s="23"/>
       <c r="O138" s="22"/>
     </row>
-    <row r="139" s="1" customFormat="1" ht="23" customHeight="1" spans="2:15">
+    <row r="139" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A139" s="19"/>
       <c r="B139" s="30" t="s">
-        <v>901</v>
+        <v>952</v>
       </c>
       <c r="C139" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D139" s="27" t="s">
-        <v>620</v>
-      </c>
-      <c r="E139" s="27"/>
+        <v>363</v>
+      </c>
+      <c r="E139" s="27" t="s">
+        <v>949</v>
+      </c>
       <c r="F139" s="27"/>
       <c r="G139" s="27"/>
       <c r="H139" s="27"/>
@@ -14004,24 +14049,20 @@
       <c r="O139" s="22"/>
     </row>
     <row r="140" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A140" s="19" t="s">
-        <v>947</v>
-      </c>
+      <c r="A140" s="19"/>
       <c r="B140" s="30" t="s">
-        <v>867</v>
-      </c>
-      <c r="C140" s="33" t="s">
+        <v>953</v>
+      </c>
+      <c r="C140" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D140" s="34" t="s">
-        <v>707</v>
-      </c>
-      <c r="E140" s="34" t="s">
-        <v>767</v>
-      </c>
-      <c r="F140" s="47" t="s">
-        <v>803</v>
-      </c>
+      <c r="D140" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E140" s="27" t="s">
+        <v>954</v>
+      </c>
+      <c r="F140" s="27"/>
       <c r="G140" s="27"/>
       <c r="H140" s="27"/>
       <c r="I140" s="27"/>
@@ -14032,19 +14073,19 @@
       <c r="N140" s="23"/>
       <c r="O140" s="22"/>
     </row>
-    <row r="141" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A141" s="19"/>
+    <row r="141" s="1" customFormat="1" ht="71" customHeight="1" spans="1:15">
+      <c r="A141" s="31"/>
       <c r="B141" s="30" t="s">
-        <v>948</v>
+        <v>955</v>
       </c>
       <c r="C141" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D141" s="27" t="s">
-        <v>600</v>
+        <v>253</v>
       </c>
       <c r="E141" s="27" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
       <c r="F141" s="27"/>
       <c r="G141" s="27"/>
@@ -14059,19 +14100,21 @@
     </row>
     <row r="142" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A142" s="19"/>
-      <c r="B142" s="30" t="s">
-        <v>950</v>
-      </c>
-      <c r="C142" s="26" t="s">
+      <c r="B142" s="62" t="s">
+        <v>833</v>
+      </c>
+      <c r="C142" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="D142" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="E142" s="27" t="s">
-        <v>951</v>
-      </c>
-      <c r="F142" s="27"/>
+      <c r="D142" s="64" t="s">
+        <v>493</v>
+      </c>
+      <c r="E142" s="64" t="s">
+        <v>957</v>
+      </c>
+      <c r="F142" s="65" t="s">
+        <v>835</v>
+      </c>
       <c r="G142" s="27"/>
       <c r="H142" s="27"/>
       <c r="I142" s="27"/>
@@ -14084,19 +14127,21 @@
     </row>
     <row r="143" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A143" s="19"/>
-      <c r="B143" s="30" t="s">
-        <v>952</v>
-      </c>
-      <c r="C143" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D143" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E143" s="27" t="s">
-        <v>949</v>
-      </c>
-      <c r="F143" s="27"/>
+      <c r="B143" s="62" t="s">
+        <v>836</v>
+      </c>
+      <c r="C143" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D143" s="64" t="s">
+        <v>471</v>
+      </c>
+      <c r="E143" s="64" t="s">
+        <v>958</v>
+      </c>
+      <c r="F143" s="64" t="s">
+        <v>959</v>
+      </c>
       <c r="G143" s="27"/>
       <c r="H143" s="27"/>
       <c r="I143" s="27"/>
@@ -14109,19 +14154,21 @@
     </row>
     <row r="144" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A144" s="19"/>
-      <c r="B144" s="30" t="s">
-        <v>953</v>
-      </c>
-      <c r="C144" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D144" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E144" s="27" t="s">
-        <v>954</v>
-      </c>
-      <c r="F144" s="27"/>
+      <c r="B144" s="62" t="s">
+        <v>839</v>
+      </c>
+      <c r="C144" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E144" s="64" t="s">
+        <v>960</v>
+      </c>
+      <c r="F144" s="64" t="s">
+        <v>961</v>
+      </c>
       <c r="G144" s="27"/>
       <c r="H144" s="27"/>
       <c r="I144" s="27"/>
@@ -14132,20 +14179,18 @@
       <c r="N144" s="23"/>
       <c r="O144" s="22"/>
     </row>
-    <row r="145" s="1" customFormat="1" ht="71" customHeight="1" spans="1:15">
-      <c r="A145" s="31"/>
+    <row r="145" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A145" s="19"/>
       <c r="B145" s="30" t="s">
-        <v>955</v>
+        <v>786</v>
       </c>
       <c r="C145" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D145" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="E145" s="27" t="s">
-        <v>956</v>
-      </c>
+        <v>638</v>
+      </c>
+      <c r="E145" s="27"/>
       <c r="F145" s="27"/>
       <c r="G145" s="27"/>
       <c r="H145" s="27"/>
@@ -14159,21 +14204,11 @@
     </row>
     <row r="146" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A146" s="19"/>
-      <c r="B146" s="62" t="s">
-        <v>833</v>
-      </c>
-      <c r="C146" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="D146" s="64" t="s">
-        <v>493</v>
-      </c>
-      <c r="E146" s="64" t="s">
-        <v>957</v>
-      </c>
-      <c r="F146" s="65" t="s">
-        <v>835</v>
-      </c>
+      <c r="B146" s="30"/>
+      <c r="C146" s="26"/>
+      <c r="D146" s="27"/>
+      <c r="E146" s="27"/>
+      <c r="F146" s="27"/>
       <c r="G146" s="27"/>
       <c r="H146" s="27"/>
       <c r="I146" s="27"/>
@@ -14186,21 +14221,11 @@
     </row>
     <row r="147" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A147" s="19"/>
-      <c r="B147" s="62" t="s">
-        <v>836</v>
-      </c>
-      <c r="C147" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D147" s="64" t="s">
-        <v>471</v>
-      </c>
-      <c r="E147" s="64" t="s">
-        <v>958</v>
-      </c>
-      <c r="F147" s="64" t="s">
-        <v>959</v>
-      </c>
+      <c r="B147" s="30"/>
+      <c r="C147" s="26"/>
+      <c r="D147" s="27"/>
+      <c r="E147" s="27"/>
+      <c r="F147" s="27"/>
       <c r="G147" s="27"/>
       <c r="H147" s="27"/>
       <c r="I147" s="27"/>
@@ -14213,21 +14238,11 @@
     </row>
     <row r="148" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A148" s="19"/>
-      <c r="B148" s="62" t="s">
-        <v>839</v>
-      </c>
-      <c r="C148" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D148" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="E148" s="64" t="s">
-        <v>960</v>
-      </c>
-      <c r="F148" s="64" t="s">
-        <v>961</v>
-      </c>
+      <c r="B148" s="30"/>
+      <c r="C148" s="26"/>
+      <c r="D148" s="27"/>
+      <c r="E148" s="27"/>
+      <c r="F148" s="27"/>
       <c r="G148" s="27"/>
       <c r="H148" s="27"/>
       <c r="I148" s="27"/>
@@ -14240,15 +14255,9 @@
     </row>
     <row r="149" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A149" s="19"/>
-      <c r="B149" s="30" t="s">
-        <v>786</v>
-      </c>
-      <c r="C149" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D149" s="27" t="s">
-        <v>638</v>
-      </c>
+      <c r="B149" s="30"/>
+      <c r="C149" s="26"/>
+      <c r="D149" s="27"/>
       <c r="E149" s="27"/>
       <c r="F149" s="27"/>
       <c r="G149" s="27"/>
@@ -14263,7 +14272,7 @@
     </row>
     <row r="150" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A150" s="19"/>
-      <c r="B150" s="30"/>
+      <c r="B150" s="20"/>
       <c r="C150" s="26"/>
       <c r="D150" s="27"/>
       <c r="E150" s="27"/>
@@ -14280,7 +14289,7 @@
     </row>
     <row r="151" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A151" s="19"/>
-      <c r="B151" s="30"/>
+      <c r="B151" s="20"/>
       <c r="C151" s="26"/>
       <c r="D151" s="27"/>
       <c r="E151" s="27"/>
@@ -14297,7 +14306,7 @@
     </row>
     <row r="152" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A152" s="19"/>
-      <c r="B152" s="30"/>
+      <c r="B152" s="20"/>
       <c r="C152" s="26"/>
       <c r="D152" s="27"/>
       <c r="E152" s="27"/>
@@ -14314,7 +14323,7 @@
     </row>
     <row r="153" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A153" s="19"/>
-      <c r="B153" s="30"/>
+      <c r="B153" s="20"/>
       <c r="C153" s="26"/>
       <c r="D153" s="27"/>
       <c r="E153" s="27"/>
@@ -15757,74 +15766,6 @@
       <c r="N237" s="23"/>
       <c r="O237" s="22"/>
     </row>
-    <row r="238" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A238" s="19"/>
-      <c r="B238" s="20"/>
-      <c r="C238" s="26"/>
-      <c r="D238" s="27"/>
-      <c r="E238" s="27"/>
-      <c r="F238" s="27"/>
-      <c r="G238" s="27"/>
-      <c r="H238" s="27"/>
-      <c r="I238" s="27"/>
-      <c r="J238" s="61"/>
-      <c r="K238" s="22"/>
-      <c r="L238" s="23"/>
-      <c r="M238" s="21"/>
-      <c r="N238" s="23"/>
-      <c r="O238" s="22"/>
-    </row>
-    <row r="239" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A239" s="19"/>
-      <c r="B239" s="20"/>
-      <c r="C239" s="26"/>
-      <c r="D239" s="27"/>
-      <c r="E239" s="27"/>
-      <c r="F239" s="27"/>
-      <c r="G239" s="27"/>
-      <c r="H239" s="27"/>
-      <c r="I239" s="27"/>
-      <c r="J239" s="61"/>
-      <c r="K239" s="22"/>
-      <c r="L239" s="23"/>
-      <c r="M239" s="21"/>
-      <c r="N239" s="23"/>
-      <c r="O239" s="22"/>
-    </row>
-    <row r="240" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A240" s="19"/>
-      <c r="B240" s="20"/>
-      <c r="C240" s="26"/>
-      <c r="D240" s="27"/>
-      <c r="E240" s="27"/>
-      <c r="F240" s="27"/>
-      <c r="G240" s="27"/>
-      <c r="H240" s="27"/>
-      <c r="I240" s="27"/>
-      <c r="J240" s="61"/>
-      <c r="K240" s="22"/>
-      <c r="L240" s="23"/>
-      <c r="M240" s="21"/>
-      <c r="N240" s="23"/>
-      <c r="O240" s="22"/>
-    </row>
-    <row r="241" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A241" s="19"/>
-      <c r="B241" s="20"/>
-      <c r="C241" s="26"/>
-      <c r="D241" s="27"/>
-      <c r="E241" s="27"/>
-      <c r="F241" s="27"/>
-      <c r="G241" s="27"/>
-      <c r="H241" s="27"/>
-      <c r="I241" s="27"/>
-      <c r="J241" s="61"/>
-      <c r="K241" s="22"/>
-      <c r="L241" s="23"/>
-      <c r="M241" s="21"/>
-      <c r="N241" s="23"/>
-      <c r="O241" s="22"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
@@ -15832,18 +15773,18 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N154:N241">
+  <conditionalFormatting sqref="N150:N237">
     <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N154,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N150,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N154,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N150,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N154,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N150,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N3:N153">
+  <conditionalFormatting sqref="N1 N3:N149">
     <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -15855,10 +15796,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C15 C16 C17 C18 C21 C22 C23 C24 C25 C26 C27 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C98 C99 C109 C110 C111 C112 C113 C114 C117 C118 C119 C120 C121 C122 C123 C124 C125 C126 C127 C128 C129 C130 C131 C132 C133 C134 C135 C136 C137 C138 C139 C140 C143 C144 C145 C146 C147 C148 C149 C13:C14 C19:C20 C28:C29 C96:C97 C100:C108 C115:C116 C141:C142 C150:C153 C154:C241">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C15 C16 C17 C18 C21 C22 C23 C24 C25 C26 C27 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C99 C105 C106 C107 C108 C109 C110 C113 C114 C115 C116 C117 C118 C119 C120 C121 C122 C123 C124 C125 C126 C127 C128 C129 C130 C131 C132 C133 C134 C135 C136 C139 C140 C141 C142 C143 C144 C145 C13:C14 C19:C20 C28:C29 C97:C98 C100:C104 C111:C112 C137:C138 C146:C149 C150:C237">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D15 D16 D17 D18 D21 D22 D23 D24 D25 D26 D27 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D98 D99 D109 D110 D111 D112 D113 D114 D117 D118 D119 D120 D121 D122 D123 D124 D125 D126 D127 D128 D129 D130 D131 D132 D133 D134 D135 D136 D137 D138 D139 D140 D143 D144 D145 D146 D147 D148 D149 D13:D14 D19:D20 D28:D29 D96:D97 D100:D108 D115:D116 D141:D142 D150:D153 D154:D241">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D15 D16 D17 D18 D21 D22 D23 D24 D25 D26 D27 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D99 D105 D106 D107 D108 D109 D110 D113 D114 D115 D116 D117 D118 D119 D120 D121 D122 D123 D124 D125 D126 D127 D128 D129 D130 D131 D132 D133 D134 D135 D136 D139 D140 D141 D142 D143 D144 D145 D13:D14 D19:D20 D28:D29 D97:D98 D100:D104 D111:D112 D137:D138 D146:D149 D150:D237">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>